<commit_message>
added Nfrond, Changed items in code for farm3D case
Firstly: the erosion rate should be proportional to the frond area/m2 segment, and not total area in a segment, since the mass is per m2 and the net growth is multiplied by the mass to get the flux per m2.

Secondly, the N uptake is way too high, as the local flux is not corrected for surface. This was fixed in FLMALN and FLMALC

The actual Velocity computed by VELOC was tied to FLMALN in process library

A final big change: I eliminated the need for the user to prescribe LinDenMAL and MALS0 based on the farm configuration/density. Instead I ask them to specify Nfrond/m2 and the correction on LinDenMAL and MALS0 is done in the code in FLMALS and MALDIS. I am not entirely confident there are no other repercussions, but the Broch test case was unaffected by these changes.
</commit_message>
<xml_diff>
--- a/documentation/calculations.xlsx
+++ b/documentation/calculations.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\MALG\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\IMPAQT\MALG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E266401C-072C-44E2-8DF1-DBD36809309D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="growth rate" sheetId="1" r:id="rId1"/>
-    <sheet name="Broch initials" sheetId="2" r:id="rId2"/>
+    <sheet name="tidal condition" sheetId="3" r:id="rId2"/>
+    <sheet name="Broch initials" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>umax</t>
   </si>
@@ -110,11 +112,35 @@
   <si>
     <t>m2</t>
   </si>
+  <si>
+    <t>mrtMAL</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>desired speed</t>
+  </si>
+  <si>
+    <t>length of domain</t>
+  </si>
+  <si>
+    <t>time to cross</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +190,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -178,7 +204,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>density limitation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -204,7 +254,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -236,256 +286,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>754</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>755</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>756</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>757</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>758</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>759</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23</c:v>
+                  <c:v>761</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>762</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27</c:v>
+                  <c:v>763</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29</c:v>
+                  <c:v>764</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31</c:v>
+                  <c:v>765</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>33</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>34</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35</c:v>
+                  <c:v>767</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37</c:v>
+                  <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>39</c:v>
+                  <c:v>769</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>40</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41</c:v>
+                  <c:v>770</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>45</c:v>
+                  <c:v>772</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>46</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>47</c:v>
+                  <c:v>773</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>48</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>49</c:v>
+                  <c:v>774</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>50</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>51</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>52</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>53</c:v>
+                  <c:v>776</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>54</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>55</c:v>
+                  <c:v>777</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>56</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>57</c:v>
+                  <c:v>778</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>58</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>59</c:v>
+                  <c:v>779</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>60</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>61</c:v>
+                  <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>62</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>63</c:v>
+                  <c:v>781</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>64</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>65</c:v>
+                  <c:v>782</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>66</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>67</c:v>
+                  <c:v>783</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>68</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>69</c:v>
+                  <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>70</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>71</c:v>
+                  <c:v>785</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>72</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>73</c:v>
+                  <c:v>786</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>74</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>75</c:v>
+                  <c:v>787</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>76</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>77</c:v>
+                  <c:v>788</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>78</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>79</c:v>
+                  <c:v>789</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>80</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>81</c:v>
+                  <c:v>790</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>82</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>83</c:v>
+                  <c:v>791</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>84</c:v>
+                  <c:v>751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,115 +547,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>0.13552758576712379</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12709006587435911</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11449988496324742</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9568072144650077E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.4179669063021462E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9914919367101494E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7816769600475729E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8337944721558168E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1435815864962283E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6746152856399615E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3764590392607985E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1987246819427655E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0992335253669425E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0468745982939204E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0209454273780707E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0088534680105326E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0035400561237647E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.0013389963743402E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0004790944981832E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0001621569229937E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0000519185237044E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.0000157246759255E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.0000045051950815E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.0000012210066457E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.0000003130365025E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.0000000759179489E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0000000174167242E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.000000003779732E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.00000000077594E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.0000000001506842E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.0000000000276809E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0000000000048103E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0000000000007906E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.0000000000001227E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.0000000000000179E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.0000000000000023E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.0000000000000002E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0.03</c:v>
@@ -752,6 +802,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5AD7-4AB0-ABEB-F54F77BF4156}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -819,7 +874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440089160"/>
@@ -881,7 +936,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440087592"/>
@@ -922,7 +977,799 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'growth rate'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erosion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'growth rate'!$E$2:$E$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>759</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>781</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>783</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>787</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>791</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'growth rate'!$G$2:$G$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E422-4F1C-AB1C-7277ACC3A2F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="774260368"/>
+        <c:axId val="774261024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="774260368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="774261024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="774261024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="774260368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -973,6 +1820,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1489,24 +2376,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1516,6 +2925,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{764C05FA-7863-496F-A511-E569C1396B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1786,17 +3231,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1821,19 +3267,15 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>750</v>
       </c>
       <c r="F2">
         <f>$B$11*EXP(-1*(E2/6)^2) + $B$12</f>
-        <v>0.13552758576712379</v>
+        <v>0.03</v>
       </c>
       <c r="G2">
-        <f>((10^-6)*EXP(0.22*E2))/(1+((10^-6)*(EXP(0.22*E2)-1)))</f>
-        <v>1.2460764239569684E-6</v>
-      </c>
-      <c r="H2">
-        <f>-1*(E2/6)^2</f>
-        <v>-2.7777777777777776E-2</v>
+        <f>((10^-6)*EXP($B$15*E2))/(1+((10^-6)*(EXP($B$15*E2)-1)))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1845,15 +3287,16 @@
         <v>0.54545454545454541</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F66" si="0">$B$11*EXP(-1*(E3/6)^2) + $B$12</f>
-        <v>0.12709006587435911</v>
+        <v>0.03</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="1">((10^-6)*EXP(0.22*E3))/(1+((10^-6)*(EXP(0.22*E3)-1)))</f>
-        <v>1.5527063603193225E-6</v>
+        <f>((10^-6)*EXP($B$15*E3))/(1+((10^-6)*(EXP($B$15*E3)-1)))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1864,15 +3307,15 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>751</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.11449988496324742</v>
+        <v>0.03</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>1.9347905257746793E-6</v>
+        <f t="shared" ref="G4:G67" si="1">((10^-6)*EXP($B$15*E4))/(1+((10^-6)*(EXP($B$15*E4)-1)))</f>
+        <v>1</v>
       </c>
       <c r="T4">
         <v>10</v>
@@ -1887,15 +3330,16 @@
         <v>0.03</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>9.9568072144650077E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>2.4108963048843208E-6</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <v>11</v>
@@ -1910,15 +3354,15 @@
         <v>3.2727272727272723E-2</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>752</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>8.4179669063021462E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>3.0041600031110242E-6</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <v>12</v>
@@ -1926,15 +3370,16 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E7">
-        <v>6</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>6.9914919367101494E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>3.7434111075068067E-6</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <v>13</v>
@@ -1949,15 +3394,15 @@
         <v>3.9E-2</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>753</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>5.7816769600475729E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>4.664573177238642E-6</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>14</v>
@@ -1972,15 +3417,16 @@
         <v>6.272727272727277E-3</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>4.8337944721558168E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>5.8124094225461322E-6</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <v>15</v>
@@ -1992,15 +3438,15 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10">
-        <v>9</v>
+        <v>754</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>4.1435815864962283E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>7.2426977708603088E-6</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <v>16</v>
@@ -2018,15 +3464,16 @@
         <v>0.1085</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>3.6746152856399615E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>9.02494107416017E-6</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>17</v>
@@ -2044,15 +3491,15 @@
         <v>0.03</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>755</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>3.3764590392607985E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.1245744092569978E-5</v>
+        <v>1</v>
       </c>
       <c r="T12">
         <v>18</v>
@@ -2067,15 +3514,16 @@
         <v>3.5749999999999997E-2</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>3.1987246819427655E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>1.4013021253434884E-5</v>
+        <v>1</v>
       </c>
       <c r="T13">
         <v>19</v>
@@ -2087,343 +3535,354 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E14">
-        <v>13</v>
+        <v>756</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>3.0992335253669425E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>1.7461239497915648E-5</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
       <c r="E15">
-        <v>14</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.0468745982939204E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>2.1757950735900389E-5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E16">
-        <v>15</v>
+        <v>757</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>3.0209454273780707E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2.7111930956594368E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17">
-        <v>16</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>3.0088534680105326E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>3.3783320896982345E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18">
-        <v>17</v>
+        <v>758</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>3.0035400561237647E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>4.2096260093313604E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19">
-        <v>18</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>3.0013389963743402E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>5.2454626774271586E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20">
-        <v>19</v>
+        <v>759</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>3.0004790944981832E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>6.5361646155887598E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21">
-        <v>20</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>3.0001621569229937E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>8.1444316398966016E-5</v>
-      </c>
-    </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22">
-        <v>21</v>
+        <v>760</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>3.0000519185237044E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>1.0148383360991019E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23">
-        <v>22</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>3.0000157246759255E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>1.2645348569324084E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24">
-        <v>23</v>
+        <v>761</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>3.0000045051950815E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>1.575658430066555E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25">
-        <v>24</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>3.0000012210066457E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>1.9633151808758198E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26">
-        <v>25</v>
+        <v>762</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>3.0000003130365025E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>2.4463231734211298E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E27">
-        <v>26</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>3.0000000759179489E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>3.0481228900170317E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E28">
-        <v>27</v>
+        <v>763</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>3.0000000174167242E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>3.797910134572184E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E29">
-        <v>28</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>3.000000003779732E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>4.7320451973457343E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E30">
-        <v>29</v>
+        <v>764</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>3.00000000077594E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>5.8958048737355951E-4</v>
-      </c>
-      <c r="M30">
-        <f>EXP(-2)</f>
-        <v>0.1353352832366127</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E31">
-        <v>30</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>3.0000000001506842E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>7.3455595524899526E-4</v>
-      </c>
-      <c r="M31">
-        <f>EXP(-3)</f>
-        <v>4.9787068367863944E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E32">
-        <v>31</v>
+        <v>765</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>3.0000000000276809E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>9.151476636868655E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33">
-        <v>32</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>3.0000000000048103E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>1.1400874650133936E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34">
-        <v>33</v>
+        <v>766</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>3.0000000000007906E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>1.4202380146384928E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35">
-        <v>34</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>3.0000000000001227E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>1.7691072610144698E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36">
-        <v>35</v>
+        <v>767</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>3.0000000000000179E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>2.2034841356053255E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37">
-        <v>36</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>3.0000000000000023E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>2.7442223184334274E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38">
-        <v>37</v>
+        <v>768</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>3.0000000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>3.417203973429205E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39">
-        <v>38</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -2431,12 +3890,12 @@
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>4.2545207523640933E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40">
-        <v>39</v>
+        <v>769</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
@@ -2444,12 +3903,13 @@
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>5.2959148119110623E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41">
-        <v>40</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -2457,12 +3917,12 @@
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>6.5905274297065781E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42">
-        <v>41</v>
+        <v>770</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
@@ -2470,12 +3930,13 @@
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>8.1990059259894974E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43">
-        <v>42</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
@@ -2483,12 +3944,12 @@
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>1.0196019167352289E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44">
-        <v>43</v>
+        <v>771</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
@@ -2496,12 +3957,13 @@
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
-        <v>1.2673225068561876E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45">
-        <v>44</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
@@ -2509,12 +3971,12 @@
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>1.5742715849473732E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46">
-        <v>45</v>
+        <v>772</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
@@ -2522,12 +3984,13 @@
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
-        <v>1.9540931966364361E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47">
-        <v>46</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
@@ -2535,12 +3998,12 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>2.4232974694841723E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48">
-        <v>47</v>
+        <v>773</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
@@ -2548,12 +4011,13 @@
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>3.0017148485242659E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49">
-        <v>48</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
@@ -2561,12 +4025,12 @@
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>3.7129413028744424E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50">
-        <v>49</v>
+        <v>774</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
@@ -2574,12 +4038,13 @@
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
-        <v>4.5847206134766547E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51">
-        <v>50</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
@@ -2587,12 +4052,12 @@
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
-        <v>5.6491800158557842E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52">
-        <v>51</v>
+        <v>775</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
@@ -2600,12 +4065,13 @@
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
-        <v>6.9427977291689119E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53">
-        <v>52</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
@@ -2613,12 +4079,12 @@
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
-        <v>8.5059380638517298E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54">
-        <v>53</v>
+        <v>776</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
@@ -2626,12 +4092,13 @@
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
-        <v>0.103817496960946</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55">
-        <v>54</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
@@ -2639,12 +4106,12 @@
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
-        <v>0.12614200844224446</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56">
-        <v>55</v>
+        <v>777</v>
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
@@ -2652,12 +4119,13 @@
       </c>
       <c r="G56">
         <f t="shared" si="1"/>
-        <v>0.15245046556210873</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57">
-        <v>56</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
@@ -2665,12 +4133,12 @@
       </c>
       <c r="G57">
         <f t="shared" si="1"/>
-        <v>0.18309621261292608</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58">
-        <v>57</v>
+        <v>778</v>
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
@@ -2678,12 +4146,13 @@
       </c>
       <c r="G58">
         <f t="shared" si="1"/>
-        <v>0.21831556557294363</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59">
-        <v>58</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
@@ -2691,12 +4160,12 @@
       </c>
       <c r="G59">
         <f t="shared" si="1"/>
-        <v>0.25816851875854974</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60">
-        <v>59</v>
+        <v>779</v>
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
@@ -2704,12 +4173,13 @@
       </c>
       <c r="G60">
         <f t="shared" si="1"/>
-        <v>0.30248136499012307</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61">
-        <v>60</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
@@ -2717,12 +4187,12 @@
       </c>
       <c r="G61">
         <f t="shared" si="1"/>
-        <v>0.35080342001031367</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62">
-        <v>61</v>
+        <v>780</v>
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
@@ -2730,12 +4200,13 @@
       </c>
       <c r="G62">
         <f t="shared" si="1"/>
-        <v>0.40239169334299929</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63">
-        <v>62</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
@@ -2743,12 +4214,12 @@
       </c>
       <c r="G63">
         <f t="shared" si="1"/>
-        <v>0.45623489645483883</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64">
-        <v>63</v>
+        <v>781</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
@@ -2756,12 +4227,13 @@
       </c>
       <c r="G64">
         <f t="shared" si="1"/>
-        <v>0.5111207761980614</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65">
-        <v>64</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
@@ -2769,12 +4241,12 @@
       </c>
       <c r="G65">
         <f t="shared" si="1"/>
-        <v>0.5657398197694945</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66">
-        <v>65</v>
+        <v>782</v>
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
@@ -2782,38 +4254,40 @@
       </c>
       <c r="G66">
         <f t="shared" si="1"/>
-        <v>0.61880766513186025</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67">
-        <v>66</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F85" si="3">$B$11*EXP(-1*(E67/6)^2) + $B$12</f>
         <v>0.03</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G85" si="4">((10^-6)*EXP(0.22*E67))/(1+((10^-6)*(EXP(0.22*E67)-1)))</f>
-        <v>0.66918260796547002</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68">
-        <v>67</v>
+        <v>783</v>
       </c>
       <c r="F68">
         <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
-        <v>0.71595618002018357</v>
+        <f t="shared" ref="G68:G85" si="4">((10^-6)*EXP($B$15*E68))/(1+((10^-6)*(EXP($B$15*E68)-1)))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69">
-        <v>68</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F69">
         <f t="shared" si="3"/>
@@ -2821,12 +4295,12 @@
       </c>
       <c r="G69">
         <f t="shared" si="4"/>
-        <v>0.75850313531882596</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70">
-        <v>69</v>
+        <v>784</v>
       </c>
       <c r="F70">
         <f t="shared" si="3"/>
@@ -2834,12 +4308,13 @@
       </c>
       <c r="G70">
         <f t="shared" si="4"/>
-        <v>0.79648854300365435</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71">
-        <v>70</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F71">
         <f t="shared" si="3"/>
@@ -2847,12 +4322,12 @@
       </c>
       <c r="G71">
         <f t="shared" si="4"/>
-        <v>0.82983953427592239</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72">
-        <v>71</v>
+        <v>785</v>
       </c>
       <c r="F72">
         <f t="shared" si="3"/>
@@ -2860,12 +4335,13 @@
       </c>
       <c r="G72">
         <f t="shared" si="4"/>
-        <v>0.85869467504450392</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73">
-        <v>72</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F73">
         <f t="shared" si="3"/>
@@ -2873,12 +4349,12 @@
       </c>
       <c r="G73">
         <f t="shared" si="4"/>
-        <v>0.88334453269096114</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74">
-        <v>73</v>
+        <v>786</v>
       </c>
       <c r="F74">
         <f t="shared" si="3"/>
@@ -2886,12 +4362,13 @@
       </c>
       <c r="G74">
         <f t="shared" si="4"/>
-        <v>0.9041742312675316</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75">
-        <v>74</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F75">
         <f t="shared" si="3"/>
@@ -2899,12 +4376,12 @@
       </c>
       <c r="G75">
         <f t="shared" si="4"/>
-        <v>0.92161467193268898</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76">
-        <v>75</v>
+        <v>787</v>
       </c>
       <c r="F76">
         <f t="shared" si="3"/>
@@ -2912,12 +4389,13 @@
       </c>
       <c r="G76">
         <f t="shared" si="4"/>
-        <v>0.93610523347285957</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77">
-        <v>76</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F77">
         <f t="shared" si="3"/>
@@ -2925,12 +4403,12 @@
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
-        <v>0.94806796961673001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78">
-        <v>77</v>
+        <v>788</v>
       </c>
       <c r="F78">
         <f t="shared" si="3"/>
@@ -2938,12 +4416,13 @@
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
-        <v>0.95789172377246945</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79">
-        <v>78</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F79">
         <f t="shared" si="3"/>
@@ -2951,12 +4430,12 @@
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
-        <v>0.96592395424992794</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80">
-        <v>79</v>
+        <v>789</v>
       </c>
       <c r="F80">
         <f t="shared" si="3"/>
@@ -2964,12 +4443,13 @@
       </c>
       <c r="G80">
         <f t="shared" si="4"/>
-        <v>0.97246805988010854</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81">
-        <v>80</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F81">
         <f t="shared" si="3"/>
@@ -2977,12 +4457,12 @@
       </c>
       <c r="G81">
         <f t="shared" si="4"/>
-        <v>0.97778431291612711</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82">
-        <v>81</v>
+        <v>790</v>
       </c>
       <c r="F82">
         <f t="shared" si="3"/>
@@ -2990,12 +4470,13 @@
       </c>
       <c r="G82">
         <f t="shared" si="4"/>
-        <v>0.98209293196423986</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83">
-        <v>82</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F83">
         <f t="shared" si="3"/>
@@ -3003,12 +4484,12 @@
       </c>
       <c r="G83">
         <f t="shared" si="4"/>
-        <v>0.98557824148585549</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E84">
-        <v>83</v>
+        <v>791</v>
       </c>
       <c r="F84">
         <f t="shared" si="3"/>
@@ -3016,12 +4497,13 @@
       </c>
       <c r="G84">
         <f t="shared" si="4"/>
-        <v>0.98839321125419799</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E85">
-        <v>84</v>
+        <f>751</f>
+        <v>751</v>
       </c>
       <c r="F85">
         <f t="shared" si="3"/>
@@ -3029,17 +4511,84 @@
       </c>
       <c r="G85">
         <f t="shared" si="4"/>
-        <v>0.99066393444071343</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5B49C-5943-47B6-86EC-8F8D7DD18322}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>0.1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>3000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <f>B2/B1</f>
+        <v>30000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <f>B3/3600</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3184,5 +4733,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additional adjustments for nFrond
Tried to make TotAreMAL prevelant across all subroutines

Fixed some units in some calculations, checks are based on balance of Storage and Consumption
</commit_message>
<xml_diff>
--- a/documentation/calculations.xlsx
+++ b/documentation/calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\IMPAQT\MALG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E266401C-072C-44E2-8DF1-DBD36809309D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E07E1EBB-39C5-48F1-876E-411DA921F761}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="growth rate" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>umax</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>nFrond</t>
+  </si>
+  <si>
+    <t>MALS0</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -286,256 +292,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>751</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>751</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>751</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>752</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>751</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>753</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>751</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>754</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>751</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>755</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>751</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>756</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>751</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>757</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>751</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>758</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>751</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>759</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>751</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>760</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>751</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>761</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>751</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>762</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>751</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>763</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>751</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>764</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>751</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>765</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>751</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>766</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>751</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>767</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>751</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>768</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>751</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>769</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>751</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>770</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>751</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>771</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>751</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>772</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>751</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>773</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>751</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>774</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>751</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>775</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>751</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>776</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>751</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>777</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>751</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>778</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>751</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>779</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>751</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>780</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>751</c:v>
+                  <c:v>6.4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>781</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>751</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>782</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>751</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>783</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>751</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>784</c:v>
+                  <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>751</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>785</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>751</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>786</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>751</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>787</c:v>
+                  <c:v>7.7</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>751</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>788</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>751</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>789</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>751</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>790</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>751</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>791</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>751</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -547,256 +553,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13742040696178476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13658815563607227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13552758576712379</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13424565414802708</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13275070642509024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.03</c:v>
+                  <c:v>0.1310523866290817</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.03</c:v>
+                  <c:v>0.12916153360192825</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.03</c:v>
+                  <c:v>0.12709006587435911</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.03</c:v>
+                  <c:v>0.1248508567037751</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.03</c:v>
+                  <c:v>0.12245760110283394</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.03</c:v>
+                  <c:v>0.11992467677605372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.03</c:v>
+                  <c:v>0.11726700093311458</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.03</c:v>
+                  <c:v>0.11449988496324742</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.03</c:v>
+                  <c:v>0.11163888893568941</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.03</c:v>
+                  <c:v>0.10869967783796318</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.03</c:v>
+                  <c:v>0.10569788137870686</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.10264895906758587</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.03</c:v>
+                  <c:v>9.9568072144650077E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.03</c:v>
+                  <c:v>9.646996376900914E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.03</c:v>
+                  <c:v>9.336884869589003E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.03</c:v>
+                  <c:v>9.0278313476264305E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03</c:v>
+                  <c:v>8.7211228008670788E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03</c:v>
+                  <c:v>8.4179669063021462E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03</c:v>
+                  <c:v>8.1194856185390088E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03</c:v>
+                  <c:v>7.8267100185189106E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03</c:v>
+                  <c:v>7.5405764205618259E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03</c:v>
+                  <c:v>7.2619237188338293E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03</c:v>
+                  <c:v>6.9914919367101494E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03</c:v>
+                  <c:v>6.7299219265196636E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03</c:v>
+                  <c:v>6.4777561530186226E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03</c:v>
+                  <c:v>6.2354404818142785E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03</c:v>
+                  <c:v>6.0033268839518872E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03</c:v>
+                  <c:v>5.7816769600475729E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.03</c:v>
+                  <c:v>5.5706661817010214E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.03</c:v>
+                  <c:v>5.3703887444149515E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.03</c:v>
+                  <c:v>5.1808629247991914E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.03</c:v>
+                  <c:v>5.0020368353239336E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.03</c:v>
+                  <c:v>4.8337944721558168E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.03</c:v>
+                  <c:v>4.6759619554811921E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.03</c:v>
+                  <c:v>4.5283138669933373E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.03</c:v>
+                  <c:v>4.3905795956801622E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.03</c:v>
+                  <c:v>4.2624496104744364E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.03</c:v>
+                  <c:v>4.1435815864962283E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.03</c:v>
+                  <c:v>4.0336063203067402E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.03</c:v>
+                  <c:v>3.9321333785925471E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.03</c:v>
+                  <c:v>3.8387564338098028E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.03</c:v>
+                  <c:v>3.7530582493562364E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.03</c:v>
+                  <c:v>3.6746152856399615E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.03</c:v>
+                  <c:v>3.6030019068345916E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.03</c:v>
+                  <c:v>3.5377941760282923E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.03</c:v>
+                  <c:v>3.4785732337911018E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.03</c:v>
+                  <c:v>3.4249282618240097E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.03</c:v>
+                  <c:v>3.3764590392607985E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.03</c:v>
+                  <c:v>3.3327781043363758E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2935125384999014E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2583053936416098E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2268167859388339E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1987246819427655E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1737254039673417E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1515338826589009E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1318836848795772E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.03</c:v>
+                  <c:v>3.114526844793257E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0992335253669425E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0857915364597886E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0740057343331809E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0636973258417625E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0547030988176471E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0468745982939204E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0400772662797549E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0341895608431219E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.03</c:v>
+                  <c:v>3.02910206831759E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0247166205604453E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0209454273780707E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0177102325231311E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0149415000735067E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0125776365368648E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0105642526948452E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0088534680105326E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0074032593724067E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0061768550345758E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0051421738317471E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0042713090911076E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0035400561237647E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0029274817462193E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,7 +880,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440089160"/>
@@ -936,7 +942,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440087592"/>
@@ -977,7 +983,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1028,7 +1034,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1071,256 +1077,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>751</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>751</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>751</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>752</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>751</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>753</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>751</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>754</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>751</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>755</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>751</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>756</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>751</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>757</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>751</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>758</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>751</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>759</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>751</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>760</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>751</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>761</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>751</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>762</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>751</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>763</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>751</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>764</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>751</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>765</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>751</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>766</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>751</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>767</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>751</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>768</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>751</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>769</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>751</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>770</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>751</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>771</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>751</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>772</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>751</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>773</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>751</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>774</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>751</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>775</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>751</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>776</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>751</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>777</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>751</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>778</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>751</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>779</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>751</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>780</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>751</c:v>
+                  <c:v>6.4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>781</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>751</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>782</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>751</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>783</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>751</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>784</c:v>
+                  <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>751</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>785</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>751</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>786</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>751</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>787</c:v>
+                  <c:v>7.7</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>751</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>788</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>751</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>789</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>751</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>790</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>751</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>791</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>751</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1332,256 +1338,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0618364808850585E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0832869774511629E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.1051708018438198E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.1274967078270953E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.1502736260012397E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.1735106673749522E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.1972171270098052E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.2214024877382903E-6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>1.2460764239569684E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.2712488054962464E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>1.296929701568323E-6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>1.323129384794887E-6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>1.3498583353161757E-6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>1.3771272449830379E-6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.4049470216336824E-6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>1.4333287934568134E-6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>1.4622839134429056E-6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>1.4918239639254003E-6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>1.5219607612136275E-6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>1.5527063603193227E-6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>1.5840730597786173E-6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>1.6160734065714355E-6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>1.6487202011402641E-6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>1.682026502510304E-6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>1.7160056335130493E-6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>1.7506711861153842E-6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>1.7860370268563314E-6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>1.8221173023936183E-6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>1.8589264451622909E-6</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1</c:v>
+                  <c:v>1.8964791791476293E-6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1</c:v>
+                  <c:v>1.9347905257746793E-6</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1</c:v>
+                  <c:v>1.9738758099167502E-6</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1</c:v>
+                  <c:v>2.0137506660252866E-6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1</c:v>
+                  <c:v>2.0544310443835655E-6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1</c:v>
+                  <c:v>2.0959332174867155E-6</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1</c:v>
+                  <c:v>2.1382737865506145E-6</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1</c:v>
+                  <c:v>2.181469688152266E-6</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1</c:v>
+                  <c:v>2.2255382010043145E-6</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1</c:v>
+                  <c:v>2.2704969528663962E-6</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1</c:v>
+                  <c:v>2.3163639275961114E-6</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1</c:v>
+                  <c:v>2.3631574723424152E-6</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1</c:v>
+                  <c:v>2.4108963048843213E-6</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1</c:v>
+                  <c:v>2.4595995211178362E-6</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1</c:v>
+                  <c:v>2.5092866026941424E-6</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1</c:v>
+                  <c:v>2.5599774248120576E-6</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1</c:v>
+                  <c:v>2.6116922641679059E-6</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1</c:v>
+                  <c:v>2.6644518070659757E-6</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1</c:v>
+                  <c:v>2.7182771576928004E-6</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1</c:v>
+                  <c:v>2.7731898465585824E-6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1</c:v>
+                  <c:v>2.8292118391091264E-6</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1</c:v>
+                  <c:v>2.8863655445117311E-6</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1</c:v>
+                  <c:v>2.9446738246185524E-6</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1</c:v>
+                  <c:v>3.0041600031110242E-6</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1</c:v>
+                  <c:v>3.0648478748289845E-6</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1</c:v>
+                  <c:v>3.1267617152882546E-6</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1</c:v>
+                  <c:v>3.189926290390453E-6</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1</c:v>
+                  <c:v>3.2543668663289605E-6</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1</c:v>
+                  <c:v>3.320109219694962E-6</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1</c:v>
+                  <c:v>3.3871796477876275E-6</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1</c:v>
+                  <c:v>3.4556049791325606E-6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1</c:v>
+                  <c:v>3.5254125842126909E-6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1</c:v>
+                  <c:v>3.5966303864159431E-6</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1</c:v>
+                  <c:v>3.6692868732040209E-6</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1</c:v>
+                  <c:v>3.7434111075068067E-6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1</c:v>
+                  <c:v>3.8190327393468952E-6</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1</c:v>
+                  <c:v>3.8961820176989516E-6</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1</c:v>
+                  <c:v>3.9748898025886056E-6</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1</c:v>
+                  <c:v>4.0551875774357238E-6</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1</c:v>
+                  <c:v>4.1371074616470099E-6</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1</c:v>
+                  <c:v>4.2206822234629718E-6</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1</c:v>
+                  <c:v>4.305945293064336E-6</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1</c:v>
+                  <c:v>4.3929307759432553E-6</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1</c:v>
+                  <c:v>4.4816734665445387E-6</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1</c:v>
+                  <c:v>4.572208862182463E-6</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1</c:v>
+                  <c:v>4.664573177238642E-6</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1</c:v>
+                  <c:v>4.7588033576466913E-6</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1</c:v>
+                  <c:v>4.8549370956694638E-6</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1</c:v>
+                  <c:v>4.9530128449747404E-6</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1</c:v>
+                  <c:v>5.0530698360154467E-6</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1</c:v>
+                  <c:v>5.1551480917204981E-6</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1</c:v>
+                  <c:v>5.2592884435025975E-6</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1</c:v>
+                  <c:v>5.3655325475893233E-6</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1</c:v>
+                  <c:v>5.4739229016841123E-6</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1</c:v>
+                  <c:v>5.5845028619637242E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,7 +1665,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774261024"/>
@@ -1721,7 +1727,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774260368"/>
@@ -1769,7 +1775,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3234,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3267,15 +3273,15 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>750</v>
+        <v>0.3</v>
       </c>
       <c r="F2">
-        <f>$B$11*EXP(-1*(E2/6)^2) + $B$12</f>
-        <v>0.03</v>
+        <f>$B$11*EXP(-1*(E2/($B$14*$B$16))^2) + $B$12</f>
+        <v>0.13742040696178476</v>
       </c>
       <c r="G2">
         <f>((10^-6)*EXP($B$15*E2))/(1+((10^-6)*(EXP($B$15*E2)-1)))</f>
-        <v>1</v>
+        <v>1.0618364808850585E-6</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -3287,16 +3293,15 @@
         <v>0.54545454545454541</v>
       </c>
       <c r="E3">
-        <f>751</f>
-        <v>751</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">$B$11*EXP(-1*(E3/6)^2) + $B$12</f>
-        <v>0.03</v>
+        <f t="shared" ref="F3:F66" si="0">$B$11*EXP(-1*(E3/($B$14*$B$16))^2) + $B$12</f>
+        <v>0.13658815563607227</v>
       </c>
       <c r="G3">
         <f>((10^-6)*EXP($B$15*E3))/(1+((10^-6)*(EXP($B$15*E3)-1)))</f>
-        <v>1</v>
+        <v>1.0832869774511629E-6</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -3307,15 +3312,15 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>751</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.13552758576712379</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G67" si="1">((10^-6)*EXP($B$15*E4))/(1+((10^-6)*(EXP($B$15*E4)-1)))</f>
-        <v>1</v>
+        <v>1.1051708018438198E-6</v>
       </c>
       <c r="T4">
         <v>10</v>
@@ -3327,19 +3332,18 @@
       </c>
       <c r="B5">
         <f>MIN(F2:F85)</f>
-        <v>0.03</v>
+        <v>3.0029274817462193E-2</v>
       </c>
       <c r="E5">
-        <f>751</f>
-        <v>751</v>
+        <v>0.6</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.13424565414802708</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1274967078270953E-6</v>
       </c>
       <c r="T5">
         <v>11</v>
@@ -3351,18 +3355,18 @@
       </c>
       <c r="B6">
         <f>B5*B4*B3*B2</f>
-        <v>3.2727272727272723E-2</v>
+        <v>3.2759208891776935E-2</v>
       </c>
       <c r="E6">
-        <v>752</v>
+        <v>0.7</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.13275070642509024</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1502736260012397E-6</v>
       </c>
       <c r="T6">
         <v>12</v>
@@ -3370,16 +3374,15 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E7">
-        <f>751</f>
-        <v>751</v>
+        <v>0.8</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.1310523866290817</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1735106673749522E-6</v>
       </c>
       <c r="T7">
         <v>13</v>
@@ -3394,15 +3397,15 @@
         <v>3.9E-2</v>
       </c>
       <c r="E8">
-        <v>753</v>
+        <v>0.9</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.12916153360192825</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1972171270098052E-6</v>
       </c>
       <c r="T8">
         <v>14</v>
@@ -3414,19 +3417,18 @@
       </c>
       <c r="B9">
         <f>B8-B6</f>
-        <v>6.272727272727277E-3</v>
+        <v>6.2407911082230649E-3</v>
       </c>
       <c r="E9">
-        <f>751</f>
-        <v>751</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.12709006587435911</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.2214024877382903E-6</v>
       </c>
       <c r="T9">
         <v>15</v>
@@ -3438,15 +3440,15 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10">
-        <v>754</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.1248508567037751</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.2460764239569684E-6</v>
       </c>
       <c r="T10">
         <v>16</v>
@@ -3464,16 +3466,15 @@
         <v>0.1085</v>
       </c>
       <c r="E11">
-        <f>751</f>
-        <v>751</v>
+        <v>1.2</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.12245760110283394</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.2712488054962464E-6</v>
       </c>
       <c r="T11">
         <v>17</v>
@@ -3491,15 +3492,15 @@
         <v>0.03</v>
       </c>
       <c r="E12">
-        <v>755</v>
+        <v>1.3</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.11992467677605372</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.296929701568323E-6</v>
       </c>
       <c r="T12">
         <v>18</v>
@@ -3514,16 +3515,15 @@
         <v>3.5749999999999997E-2</v>
       </c>
       <c r="E13">
-        <f>751</f>
-        <v>751</v>
+        <v>1.4</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.11726700093311458</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.323129384794887E-6</v>
       </c>
       <c r="T13">
         <v>19</v>
@@ -3534,16 +3534,22 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>0.06</v>
+      </c>
       <c r="E14">
-        <v>756</v>
+        <v>1.5</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.11449988496324742</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.3498583353161757E-6</v>
       </c>
       <c r="T14">
         <v>20</v>
@@ -3557,961 +3563,931 @@
         <v>0.2</v>
       </c>
       <c r="E15">
-        <f>751</f>
-        <v>751</v>
+        <v>1.6</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.11163888893568941</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.3771272449830379E-6</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
       <c r="E16">
-        <v>757</v>
+        <v>1.7</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.10869967783796318</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.4049470216336824E-6</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17">
-        <f>751</f>
-        <v>751</v>
+        <v>1.8</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.10569788137870686</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.4333287934568134E-6</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18">
-        <v>758</v>
+        <v>1.9</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.10264895906758587</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.4622839134429056E-6</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19">
-        <f>751</f>
-        <v>751</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>9.9568072144650077E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.4918239639254003E-6</v>
       </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20">
-        <v>759</v>
+        <v>2.1</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>9.646996376900914E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5219607612136275E-6</v>
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21">
-        <f>751</f>
-        <v>751</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>9.336884869589003E-2</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5527063603193227E-6</v>
       </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22">
-        <v>760</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>9.0278313476264305E-2</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5840730597786173E-6</v>
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23">
-        <f>751</f>
-        <v>751</v>
+        <v>2.4</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>8.7211228008670788E-2</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.6160734065714355E-6</v>
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24">
-        <v>761</v>
+        <v>2.5</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>8.4179669063021462E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.6487202011402641E-6</v>
       </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25">
-        <f>751</f>
-        <v>751</v>
+        <v>2.6</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>8.1194856185390088E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.682026502510304E-6</v>
       </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26">
-        <v>762</v>
+        <v>2.7</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>7.8267100185189106E-2</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.7160056335130493E-6</v>
       </c>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E27">
-        <f>751</f>
-        <v>751</v>
+        <v>2.8</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>7.5405764205618259E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.7506711861153842E-6</v>
       </c>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E28">
-        <v>763</v>
+        <v>2.9</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>7.2619237188338293E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.7860370268563314E-6</v>
       </c>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E29">
-        <f>751</f>
-        <v>751</v>
+        <v>3</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>6.9914919367101494E-2</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.8221173023936183E-6</v>
       </c>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E30">
-        <v>764</v>
+        <v>3.1</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>6.7299219265196636E-2</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.8589264451622909E-6</v>
       </c>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E31">
-        <f>751</f>
-        <v>751</v>
+        <v>3.2</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>6.4777561530186226E-2</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.8964791791476293E-6</v>
       </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E32">
-        <v>765</v>
+        <v>3.3</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>6.2354404818142785E-2</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.9347905257746793E-6</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33">
-        <f>751</f>
-        <v>751</v>
+        <v>3.4</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>6.0033268839518872E-2</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.9738758099167502E-6</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34">
-        <v>766</v>
+        <v>3.5</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>5.7816769600475729E-2</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.0137506660252866E-6</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35">
-        <f>751</f>
-        <v>751</v>
+        <v>3.6</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>5.5706661817010214E-2</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.0544310443835655E-6</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36">
-        <v>767</v>
+        <v>3.7</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>5.3703887444149515E-2</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.0959332174867155E-6</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37">
-        <f>751</f>
-        <v>751</v>
+        <v>3.8</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>5.1808629247991914E-2</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.1382737865506145E-6</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38">
-        <v>768</v>
+        <v>3.9</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>5.0020368353239336E-2</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.181469688152266E-6</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39">
-        <f>751</f>
-        <v>751</v>
+        <v>4</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.8337944721558168E-2</v>
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.2255382010043145E-6</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40">
-        <v>769</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.6759619554811921E-2</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.2704969528663962E-6</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41">
-        <f>751</f>
-        <v>751</v>
+        <v>4.2</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.5283138669933373E-2</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.3163639275961114E-6</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42">
-        <v>770</v>
+        <v>4.3</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.3905795956801622E-2</v>
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.3631574723424152E-6</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43">
-        <f>751</f>
-        <v>751</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.2624496104744364E-2</v>
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.4108963048843213E-6</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44">
-        <v>771</v>
+        <v>4.5</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.1435815864962283E-2</v>
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.4595995211178362E-6</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45">
-        <f>751</f>
-        <v>751</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>4.0336063203067402E-2</v>
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5092866026941424E-6</v>
       </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46">
-        <v>772</v>
+        <v>4.7</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.9321333785925471E-2</v>
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5599774248120576E-6</v>
       </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47">
-        <f>751</f>
-        <v>751</v>
+        <v>4.8</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.8387564338098028E-2</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.6116922641679059E-6</v>
       </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48">
-        <v>773</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.7530582493562364E-2</v>
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.6644518070659757E-6</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49">
-        <f>751</f>
-        <v>751</v>
+        <v>5</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.6746152856399615E-2</v>
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.7182771576928004E-6</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50">
-        <v>774</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.6030019068345916E-2</v>
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.7731898465585824E-6</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51">
-        <f>751</f>
-        <v>751</v>
+        <v>5.2</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.5377941760282923E-2</v>
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.8292118391091264E-6</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52">
-        <v>775</v>
+        <v>5.3</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.4785732337911018E-2</v>
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.8863655445117311E-6</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53">
-        <f>751</f>
-        <v>751</v>
+        <v>5.4</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.4249282618240097E-2</v>
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.9446738246185524E-6</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54">
-        <v>776</v>
+        <v>5.5</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.3764590392607985E-2</v>
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.0041600031110242E-6</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55">
-        <f>751</f>
-        <v>751</v>
+        <v>5.6</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.3327781043363758E-2</v>
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.0648478748289845E-6</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56">
-        <v>777</v>
+        <v>5.7</v>
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.2935125384999014E-2</v>
       </c>
       <c r="G56">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.1267617152882546E-6</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57">
-        <f>751</f>
-        <v>751</v>
+        <v>5.8</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.2583053936416098E-2</v>
       </c>
       <c r="G57">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.189926290390453E-6</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58">
-        <v>778</v>
+        <v>5.9</v>
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.2268167859388339E-2</v>
       </c>
       <c r="G58">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.2543668663289605E-6</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59">
-        <f>751</f>
-        <v>751</v>
+        <v>6</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.1987246819427655E-2</v>
       </c>
       <c r="G59">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.320109219694962E-6</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60">
-        <v>779</v>
+        <v>6.1</v>
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.1737254039673417E-2</v>
       </c>
       <c r="G60">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.3871796477876275E-6</v>
       </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61">
-        <f>751</f>
-        <v>751</v>
+        <v>6.2</v>
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.1515338826589009E-2</v>
       </c>
       <c r="G61">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.4556049791325606E-6</v>
       </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62">
-        <v>780</v>
+        <v>6.3</v>
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.1318836848795772E-2</v>
       </c>
       <c r="G62">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.5254125842126909E-6</v>
       </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63">
-        <f>751</f>
-        <v>751</v>
+        <v>6.4</v>
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.114526844793257E-2</v>
       </c>
       <c r="G63">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.5966303864159431E-6</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64">
-        <v>781</v>
+        <v>6.5</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.0992335253669425E-2</v>
       </c>
       <c r="G64">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.6692868732040209E-6</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65">
-        <f>751</f>
-        <v>751</v>
+        <v>6.6</v>
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.0857915364597886E-2</v>
       </c>
       <c r="G65">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.7434111075068067E-6</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66">
-        <v>782</v>
+        <v>6.7</v>
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.0740057343331809E-2</v>
       </c>
       <c r="G66">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.8190327393468952E-6</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67">
-        <f>751</f>
-        <v>751</v>
+        <v>6.8</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F85" si="3">$B$11*EXP(-1*(E67/6)^2) + $B$12</f>
-        <v>0.03</v>
+        <f t="shared" ref="F67:F85" si="3">$B$11*EXP(-1*(E67/($B$14*$B$16))^2) + $B$12</f>
+        <v>3.0636973258417625E-2</v>
       </c>
       <c r="G67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.8961820176989516E-6</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68">
-        <v>783</v>
+        <v>6.9</v>
       </c>
       <c r="F68">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0547030988176471E-2</v>
       </c>
       <c r="G68">
         <f t="shared" ref="G68:G85" si="4">((10^-6)*EXP($B$15*E68))/(1+((10^-6)*(EXP($B$15*E68)-1)))</f>
-        <v>1</v>
+        <v>3.9748898025886056E-6</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69">
-        <f>751</f>
-        <v>751</v>
+        <v>7</v>
       </c>
       <c r="F69">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0468745982939204E-2</v>
       </c>
       <c r="G69">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.0551875774357238E-6</v>
       </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70">
-        <v>784</v>
+        <v>7.1</v>
       </c>
       <c r="F70">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0400772662797549E-2</v>
       </c>
       <c r="G70">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.1371074616470099E-6</v>
       </c>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71">
-        <f>751</f>
-        <v>751</v>
+        <v>7.2</v>
       </c>
       <c r="F71">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0341895608431219E-2</v>
       </c>
       <c r="G71">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.2206822234629718E-6</v>
       </c>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72">
-        <v>785</v>
+        <v>7.3</v>
       </c>
       <c r="F72">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.02910206831759E-2</v>
       </c>
       <c r="G72">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.305945293064336E-6</v>
       </c>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73">
-        <f>751</f>
-        <v>751</v>
+        <v>7.4</v>
       </c>
       <c r="F73">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0247166205604453E-2</v>
       </c>
       <c r="G73">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.3929307759432553E-6</v>
       </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74">
-        <v>786</v>
+        <v>7.5</v>
       </c>
       <c r="F74">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0209454273780707E-2</v>
       </c>
       <c r="G74">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.4816734665445387E-6</v>
       </c>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75">
-        <f>751</f>
-        <v>751</v>
+        <v>7.6</v>
       </c>
       <c r="F75">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0177102325231311E-2</v>
       </c>
       <c r="G75">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.572208862182463E-6</v>
       </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76">
-        <v>787</v>
+        <v>7.7</v>
       </c>
       <c r="F76">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0149415000735067E-2</v>
       </c>
       <c r="G76">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.664573177238642E-6</v>
       </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77">
-        <f>751</f>
-        <v>751</v>
+        <v>7.8</v>
       </c>
       <c r="F77">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0125776365368648E-2</v>
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.7588033576466913E-6</v>
       </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78">
-        <v>788</v>
+        <v>7.9</v>
       </c>
       <c r="F78">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0105642526948452E-2</v>
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.8549370956694638E-6</v>
       </c>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79">
-        <f>751</f>
-        <v>751</v>
+        <v>8</v>
       </c>
       <c r="F79">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0088534680105326E-2</v>
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.9530128449747404E-6</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80">
-        <v>789</v>
+        <v>8.1</v>
       </c>
       <c r="F80">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0074032593724067E-2</v>
       </c>
       <c r="G80">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.0530698360154467E-6</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81">
-        <f>751</f>
-        <v>751</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F81">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0061768550345758E-2</v>
       </c>
       <c r="G81">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.1551480917204981E-6</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82">
-        <v>790</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F82">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0051421738317471E-2</v>
       </c>
       <c r="G82">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.2592884435025975E-6</v>
       </c>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83">
-        <f>751</f>
-        <v>751</v>
+        <v>8.4</v>
       </c>
       <c r="F83">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0042713090911076E-2</v>
       </c>
       <c r="G83">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.3655325475893233E-6</v>
       </c>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E84">
-        <v>791</v>
+        <v>8.5</v>
       </c>
       <c r="F84">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0035400561237647E-2</v>
       </c>
       <c r="G84">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.4739229016841123E-6</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E85">
-        <f>751</f>
-        <v>751</v>
+        <v>8.6</v>
       </c>
       <c r="F85">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>3.0029274817462193E-2</v>
       </c>
       <c r="G85">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.5845028619637242E-6</v>
       </c>
     </row>
   </sheetData>
@@ -4525,7 +4501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5B49C-5943-47B6-86EC-8F8D7DD18322}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added flexible preference for ammonia
Also adjusted some aspects of plotting routines
</commit_message>
<xml_diff>
--- a/documentation/calculations.xlsx
+++ b/documentation/calculations.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\IMPAQT\MALG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F74D4FF-45AF-4365-9B72-0DDBA4032B04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA02008-BB35-4072-AB8B-D9D4A7D51BE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="growth rate" sheetId="1" r:id="rId1"/>
     <sheet name="tidal condition" sheetId="3" r:id="rId2"/>
     <sheet name="Broch initials" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -269,7 +275,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -301,256 +307,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>302</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>303</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>304</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>305</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>306</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>307</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>308</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>309</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>310</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>311</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>312</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>314</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>315</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>316</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>317</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>318</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>319</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>320</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>321</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>322</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>323</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>324</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>325</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>326</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>327</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>328</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>329</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>330</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>331</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>332</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>333</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>334</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>335</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>336</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>337</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>338</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>339</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>340</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>341</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>342</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>343</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>344</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>345</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>346</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>347</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>348</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>349</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>350</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>351</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>352</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>353</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>354</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>355</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>356</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>357</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>358</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>359</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>360</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>361</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>362</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>363</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>364</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>365</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>366</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>367</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>368</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>369</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>370</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>371</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>372</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>373</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>374</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>375</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>376</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>377</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>378</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>379</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>380</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>381</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>382</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>383</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,256 +568,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
+                  <c:v>0.13850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13552758576712379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12709006587435911</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11449988496324742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9568072144650063E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4179669063021462E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9914919367101494E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7816769600475729E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8337944721558161E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1435815864962283E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6746152856399615E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3764590392607978E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.1987246819427655E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0992335253669422E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0468745982939204E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3.0209454273780707E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0200892379812778E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0192653712358762E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0184727257221756E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0177102325231311E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0169768544686129E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0162715853892286E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.0155934493799167E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0149415000735067E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.0143148199244237E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.0137125195027013E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.0131337367984422E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0125776365368648E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.0120434095040369E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.0115302718834093E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.0110374646032195E-2</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0105642526948452E-2</c:v>
+                  <c:v>3.0088534680105326E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.0101099246621625E-2</c:v>
+                  <c:v>3.0035400561237647E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0096737918619481E-2</c:v>
+                  <c:v>3.0013389963743402E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0092551878953627E-2</c:v>
+                  <c:v>3.0004790944981832E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0088534680105326E-2</c:v>
+                  <c:v>3.0001621569229937E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.0084680085162376E-2</c:v>
+                  <c:v>3.0000519185237044E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.0080982062067031E-2</c:v>
+                  <c:v>3.0000157246759255E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.007743477797482E-2</c:v>
+                  <c:v>3.0000045051950815E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.0074032593724067E-2</c:v>
+                  <c:v>3.0000012210066457E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.0070770058415741E-2</c:v>
+                  <c:v>3.0000003130365025E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.006764190410325E-2</c:v>
+                  <c:v>3.0000000759179489E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.0064643040591657E-2</c:v>
+                  <c:v>3.0000000174167242E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.0061768550345758E-2</c:v>
+                  <c:v>3.000000003779732E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.0059013683506323E-2</c:v>
+                  <c:v>3.00000000077594E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.0056373853013799E-2</c:v>
+                  <c:v>3.0000000001506842E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.005384462983865E-2</c:v>
+                  <c:v>3.0000000000276809E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0051421738317471E-2</c:v>
+                  <c:v>3.0000000000048103E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.0049101051593922E-2</c:v>
+                  <c:v>3.0000000000007906E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.0046878587163543E-2</c:v>
+                  <c:v>3.0000000000001227E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.0044750502521336E-2</c:v>
+                  <c:v>3.0000000000000179E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.0042713090911076E-2</c:v>
+                  <c:v>3.0000000000000023E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.0040762777175184E-2</c:v>
+                  <c:v>3.0000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.0038896113703976E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.0037109776483065E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.0035400561237647E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.0033765379672384E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.0032201255805562E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.0030705322396111E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.0029274817462193E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.0027907080889871E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.0026599551130486E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.0025349761985259E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.0024155339475698E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.0023013998798292E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.0021923541362044E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.002088185190736E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.0019886895704707E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.0018936715831692E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.001802943052689E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.0017163230619013E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.0016336377029905E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.0015547198349812E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.0014794088483461E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.0014075504365443E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.0013389963743402E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.001273604302758E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.0012112375205166E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.0011517647818096E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.0010950601002742E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.0010410025590149E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.0009894761265303E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.0009403694784092E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>3.0008935758246504E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.0008489927424727E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.0008065220144767E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>3.0007660694720214E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>3.0007275448436854E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>3.0006908616086826E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3.0006559368550987E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3.0006226911428232E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>3.0005910483710544E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>3.0005609356502497E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>3.0005322831783997E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3.0005050241215126E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>3.0004790944981832E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>3.0004544330681383E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>3.0004309812246419E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>3.0004086828906512E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -897,7 +903,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -935,7 +941,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440089160"/>
@@ -1014,7 +1020,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1052,7 +1058,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="440087592"/>
@@ -1094,7 +1100,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1124,7 +1130,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1175,7 +1181,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1218,256 +1224,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>302</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>303</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>304</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>305</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>306</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>307</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>308</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>309</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>310</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>311</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>312</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>314</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>315</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>316</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>317</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>318</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>319</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>320</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>321</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>322</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>323</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>324</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>325</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>326</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>327</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>328</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>329</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>330</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>331</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>332</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>333</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>334</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>335</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>336</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>337</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>338</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>339</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>340</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>341</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>342</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>343</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>344</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>345</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>346</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>347</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>348</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>349</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>350</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>351</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>352</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>353</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>354</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>355</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>356</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>357</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>358</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>359</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>360</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>361</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>362</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>363</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>364</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>365</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>366</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>367</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>368</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>369</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>370</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>371</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>372</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>373</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>374</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>375</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>376</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>377</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>378</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>379</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>380</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>381</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>382</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>383</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,256 +1485,256 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2460764239569684E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5527063603193225E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9347905257746793E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4108963048843208E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0041600031110242E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7434111075068067E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.664573177238642E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8124094225461322E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2426977708603088E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.02494107416017E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1245744092569978E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4013021253434884E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7461239497915648E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1757950735900389E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2.7111930956594368E-5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7411800279662338E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7714986191239534E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.8021525371123946E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.8331454904728236E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.8644812287563976E-5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.8961635429775755E-5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.9281962660724969E-5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.9605832733624805E-5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.9933284830225933E-5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.0264358565554303E-5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.0599093992701158E-5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0937531607665947E-5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.1279712354252954E-5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.1625677629021711E-5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.1975469286292455E-5</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.232912964320662E-5</c:v>
+                  <c:v>3.3783320896982345E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2686701484843383E-5</c:v>
+                  <c:v>4.2096260093313604E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3048228069392744E-5</c:v>
+                  <c:v>5.2454626774271586E-5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3413753133385748E-5</c:v>
+                  <c:v>6.5361646155887598E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.3783320896982358E-5</c:v>
+                  <c:v>8.1444316398966016E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.4156976069318018E-5</c:v>
+                  <c:v>1.0148383360991019E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.453476385390916E-5</c:v>
+                  <c:v>1.2645348569324084E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.4916729954118298E-5</c:v>
+                  <c:v>1.575658430066555E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.5302920578679762E-5</c:v>
+                  <c:v>1.9633151808758198E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.5693382447286248E-5</c:v>
+                  <c:v>2.4463231734211298E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6088162796237222E-5</c:v>
+                  <c:v>3.0481228900170317E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.6487309384149801E-5</c:v>
+                  <c:v>3.797910134572184E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.6890870497732464E-5</c:v>
+                  <c:v>4.7320451973457343E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.7298894957622849E-5</c:v>
+                  <c:v>5.8958048737355951E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.7711432124289786E-5</c:v>
+                  <c:v>7.3455595524899526E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.8128531904000816E-5</c:v>
+                  <c:v>9.151476636868655E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.855024475485522E-5</c:v>
+                  <c:v>1.1400874650133936E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.8976621692884314E-5</c:v>
+                  <c:v>1.4202380146384928E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.9407714298218417E-5</c:v>
+                  <c:v>1.7691072610144698E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.9843574721322512E-5</c:v>
+                  <c:v>2.2034841356053255E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.0284255689300545E-5</c:v>
+                  <c:v>2.7442223184334274E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.0729810512269309E-5</c:v>
+                  <c:v>3.417203973429205E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.1180293089803006E-5</c:v>
+                  <c:v>4.2545207523640933E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.1635757917448627E-5</c:v>
+                  <c:v>5.2959148119110623E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.2096260093313591E-5</c:v>
+                  <c:v>6.5905274297065781E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.256185532472612E-5</c:v>
+                  <c:v>8.1990059259894974E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.3032599934968963E-5</c:v>
+                  <c:v>1.0196019167352289E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.3508550870087824E-5</c:v>
+                  <c:v>1.2673225068561876E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.3989765705774741E-5</c:v>
+                  <c:v>1.5742715849473732E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.4476302654327502E-5</c:v>
+                  <c:v>1.9540931966364361E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.4968220571686174E-5</c:v>
+                  <c:v>2.4232974694841723E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.5465578964547087E-5</c:v>
+                  <c:v>3.0017148485242659E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.5968437997555506E-5</c:v>
+                  <c:v>3.7129413028744424E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.6476858500577689E-5</c:v>
+                  <c:v>4.5847206134766547E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.6990901976053392E-5</c:v>
+                  <c:v>5.6491800158557842E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.7510630606429336E-5</c:v>
+                  <c:v>6.9427977291689119E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.80361072616751E-5</c:v>
+                  <c:v>8.5059380638517298E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.8567395506881678E-5</c:v>
+                  <c:v>0.103817496960946</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.9104559609944175E-5</c:v>
+                  <c:v>0.12614200844224446</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.9647664549329351E-5</c:v>
+                  <c:v>0.15245046556210873</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>5.0196776021928776E-5</c:v>
+                  <c:v>0.18309621261292608</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>5.0751960450998819E-5</c:v>
+                  <c:v>0.21831556557294363</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>5.1313284994188345E-5</c:v>
+                  <c:v>0.25816851875854974</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.1880817551655123E-5</c:v>
+                  <c:v>0.30248136499012307</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>5.2454626774271586E-5</c:v>
+                  <c:v>0.35080342001031367</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>5.3034782071921506E-5</c:v>
+                  <c:v>0.40239169334299929</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.3621353621888093E-5</c:v>
+                  <c:v>0.45623489645483883</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.4214412377334787E-5</c:v>
+                  <c:v>0.5111207761980614</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.4814030075879776E-5</c:v>
+                  <c:v>0.5657398197694945</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5.5420279248265029E-5</c:v>
+                  <c:v>0.61880766513186025</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>5.6033233227121078E-5</c:v>
+                  <c:v>0.66918260796547002</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.6652966155828694E-5</c:v>
+                  <c:v>0.71595618002018357</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.7279552997478292E-5</c:v>
+                  <c:v>0.75850313531882596</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.7913069543928314E-5</c:v>
+                  <c:v>0.79648854300365435</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.8553592424963564E-5</c:v>
+                  <c:v>0.82983953427592239</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.9201199117554711E-5</c:v>
+                  <c:v>0.85869467504450392</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5.9855967955219987E-5</c:v>
+                  <c:v>0.88334453269096114</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>6.0517978137490211E-5</c:v>
+                  <c:v>0.9041742312675316</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6.11873097394785E-5</c:v>
+                  <c:v>0.92161467193268898</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.1864043721555188E-5</c:v>
+                  <c:v>0.93610523347285957</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.2548261939129998E-5</c:v>
+                  <c:v>0.94806796961673001</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6.3240047152541973E-5</c:v>
+                  <c:v>0.95789172377246945</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>6.3939483037058633E-5</c:v>
+                  <c:v>0.96592395424992794</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.4646654192985649E-5</c:v>
+                  <c:v>0.97246805988010854</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6.5361646155887598E-5</c:v>
+                  <c:v>0.97778431291612711</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>6.6084545406922302E-5</c:v>
+                  <c:v>0.98209293196423986</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>6.6815439383288355E-5</c:v>
+                  <c:v>0.98557824148585549</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>6.7554416488789119E-5</c:v>
+                  <c:v>0.98839321125419799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1809,7 +1815,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1847,7 +1853,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774261024"/>
@@ -1926,7 +1932,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1964,7 +1970,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774260368"/>
@@ -2006,7 +2012,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2043,7 +2049,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3170,16 +3176,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>297517</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>147356</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>287991</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>42581</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3207,15 +3213,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>134751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3509,7 +3515,7 @@
   <dimension ref="A1:V85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H85"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,23 +3555,23 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>D2/100</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f>$B$11*EXP(-1*(E2/($B$14*$B$16))^2) + $B$12</f>
-        <v>3.0209454273780707E-2</v>
+        <v>0.13850000000000001</v>
       </c>
       <c r="G2">
         <f>EXP($B$15*D2)</f>
-        <v>4.6071866343312918E+28</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>((10^-6)*EXP($B$15*D2/$B$16))/(1+((10^-6)*(EXP($B$15*D2/$B$16)-1)))</f>
-        <v>2.7111930956594368E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -3577,23 +3583,23 @@
         <v>0.54545454545454541</v>
       </c>
       <c r="D3">
-        <v>301</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" si="0">D3/100</f>
-        <v>3.01</v>
+        <v>0.01</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F66" si="1">$B$11*EXP(-1*(E3/($B$14*$B$16))^2) + $B$12</f>
-        <v>3.0200892379812778E-2</v>
+        <v>0.13552758576712379</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" si="2">EXP($B$15*D3)</f>
-        <v>5.7409080585134084E+28</v>
+        <v>1.2460767305873808</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H66" si="3">((10^-6)*EXP($B$15*D3/$B$16))/(1+((10^-6)*(EXP($B$15*D3/$B$16)-1)))</f>
-        <v>2.7411800279662338E-5</v>
+        <v>1.2460764239569684E-6</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -3604,23 +3610,23 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>302</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>3.02</v>
+        <v>0.02</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>3.0192653712358762E-2</v>
+        <v>0.12709006587435911</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>7.1536119441551272E+28</v>
+        <v>1.552707218511336</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>2.7714986191239534E-5</v>
+        <v>1.5527063603193225E-6</v>
       </c>
       <c r="U4">
         <v>10</v>
@@ -3632,26 +3638,26 @@
       </c>
       <c r="B5">
         <f>MIN(F2:F85)</f>
-        <v>3.0004086828906512E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D5">
-        <v>303</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3.03</v>
+        <v>0.03</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>3.0184727257221756E-2</v>
+        <v>0.11449988496324742</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>8.9139493832636476E+28</v>
+        <v>1.9347923344020317</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>2.8021525371123946E-5</v>
+        <v>1.9347905257746793E-6</v>
       </c>
       <c r="U5">
         <v>11</v>
@@ -3663,26 +3669,26 @@
       </c>
       <c r="B6">
         <f>B5*B4*B3*B2</f>
-        <v>3.2731731086079831E-2</v>
+        <v>3.2727272727272723E-2</v>
       </c>
       <c r="D6">
-        <v>304</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>3.04</v>
+        <v>0.04</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>3.0177102325231311E-2</v>
+        <v>9.9568072144650063E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>1.1107464904118554E+29</v>
+        <v>2.4108997064172097</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>2.8331454904728236E-5</v>
+        <v>2.4108963048843208E-6</v>
       </c>
       <c r="U6">
         <v>12</v>
@@ -3690,23 +3696,23 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7">
-        <v>305</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>3.05</v>
+        <v>0.05</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>3.0169768544686129E-2</v>
+        <v>8.4179669063021462E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.3840753552838107E+29</v>
+        <v>3.0041660239464334</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>2.8644812287563976E-5</v>
+        <v>3.0041600031110242E-6</v>
       </c>
       <c r="U7">
         <v>13</v>
@@ -3721,23 +3727,23 @@
         <v>3.9E-2</v>
       </c>
       <c r="D8">
-        <v>306</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>3.06</v>
+        <v>0.06</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>3.0162715853892286E-2</v>
+        <v>6.9914919367101494E-2</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>1.7246640935986408E+29</v>
+        <v>3.7434213772608627</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>2.8961635429775755E-5</v>
+        <v>3.7434111075068067E-6</v>
       </c>
       <c r="U8">
         <v>14</v>
@@ -3749,26 +3755,26 @@
       </c>
       <c r="B9">
         <f>B8-B6</f>
-        <v>6.2682689139201692E-3</v>
+        <v>6.272727272727277E-3</v>
       </c>
       <c r="D9">
-        <v>307</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>3.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>3.0155934493799167E-2</v>
+        <v>5.7816769600475729E-2</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>2.1490637951128407E+29</v>
+        <v>4.6645902709881257</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>2.9281962660724969E-5</v>
+        <v>4.664573177238642E-6</v>
       </c>
       <c r="U9">
         <v>15</v>
@@ -3780,23 +3786,23 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10">
-        <v>308</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>3.08</v>
+        <v>0.08</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>3.0149415000735067E-2</v>
+        <v>4.8337944721558161E-2</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>2.6778983876379141E+29</v>
+        <v>5.8124373944025889</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>2.9605832733624805E-5</v>
+        <v>5.8124094225461322E-6</v>
       </c>
       <c r="U10">
         <v>16</v>
@@ -3814,23 +3820,23 @@
         <v>0.1085</v>
       </c>
       <c r="D11">
-        <v>309</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>3.09</v>
+        <v>0.09</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>3.0143148199244237E-2</v>
+        <v>4.1435815864962283E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>3.3368668677130671E+29</v>
+        <v>7.2427429851610121</v>
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>2.9933284830225933E-5</v>
+        <v>7.2426977708603088E-6</v>
       </c>
       <c r="U11">
         <v>17</v>
@@ -3848,23 +3854,23 @@
         <v>0.03</v>
       </c>
       <c r="D12">
-        <v>310</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>3.1</v>
+        <v>0.1</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>3.0137125195027013E-2</v>
+        <v>3.6746152856399615E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>4.157992156925248E+29</v>
+        <v>9.025013499434122</v>
       </c>
       <c r="H12">
         <f t="shared" si="3"/>
-        <v>3.0264358565554303E-5</v>
+        <v>9.02494107416017E-6</v>
       </c>
       <c r="U12">
         <v>18</v>
@@ -3879,23 +3885,23 @@
         <v>3.5749999999999997E-2</v>
       </c>
       <c r="D13">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>3.11</v>
+        <v>0.11</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.0131337367984422E-2</v>
+        <v>3.3764590392607978E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>5.1811772727093785E+29</v>
+        <v>11.245859314881844</v>
       </c>
       <c r="H13">
         <f t="shared" si="3"/>
-        <v>3.0599093992701158E-5</v>
+        <v>1.1245744092569978E-5</v>
       </c>
       <c r="U13">
         <v>19</v>
@@ -3913,23 +3919,23 @@
         <v>0.06</v>
       </c>
       <c r="D14">
-        <v>312</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>3.12</v>
+        <v>0.12</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>3.0125776365368648E-2</v>
+        <v>3.1987246819427655E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>6.4561444365713378E+29</v>
+        <v>14.013203607733615</v>
       </c>
       <c r="H14">
         <f t="shared" si="3"/>
-        <v>3.0937531607665947E-5</v>
+        <v>1.4013021253434884E-5</v>
       </c>
       <c r="U14">
         <v>20</v>
@@ -3943,23 +3949,23 @@
         <v>0.22</v>
       </c>
       <c r="D15">
-        <v>313</v>
+        <v>13</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>3.13</v>
+        <v>0.13</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>3.0120434095040369E-2</v>
+        <v>3.0992335253669422E-2</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>8.0448513517227109E+29</v>
+        <v>17.46152693657999</v>
       </c>
       <c r="H15">
         <f t="shared" si="3"/>
-        <v>3.1279712354252954E-5</v>
+        <v>1.7461239497915648E-5</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -3967,1475 +3973,1475 @@
         <v>36</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>314</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>3.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>3.0115302718834093E-2</v>
+        <v>3.0468745982939204E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>1.0024502070416096E+30</v>
+        <v>21.758402396197081</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>3.1625677629021711E-5</v>
+        <v>2.1757950735900389E-5</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17">
-        <v>315</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>0.15</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>3.0110374646032195E-2</v>
+        <v>3.0209454273780707E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>1.2491298765670503E+30</v>
+        <v>27.112638920657883</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>3.1975469286292455E-5</v>
+        <v>2.7111930956594368E-5</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18">
-        <v>316</v>
+        <v>16</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>3.16</v>
+        <v>0.16</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>3.0105642526948452E-2</v>
+        <v>3.0088534680105326E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>1.5565116726716869E+30</v>
+        <v>33.784428463849558</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
-        <v>3.232912964320662E-5</v>
+        <v>3.3783320896982345E-5</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19">
-        <v>317</v>
+        <v>17</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>3.17</v>
+        <v>0.17</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.0101099246621625E-2</v>
+        <v>3.0035400561237647E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>1.9395329762038288E+30</v>
+        <v>42.097990164996908</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>3.2686701484843383E-5</v>
+        <v>4.2096260093313604E-5</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20">
-        <v>318</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>3.18</v>
+        <v>0.18</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>3.0096737918619481E-2</v>
+        <v>3.0013389963743402E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>2.4168069098544765E+30</v>
+        <v>52.457325949099051</v>
       </c>
       <c r="H20">
         <f t="shared" si="3"/>
-        <v>3.3048228069392744E-5</v>
+        <v>5.2454626774271586E-5</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21">
-        <v>319</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>3.19</v>
+        <v>0.19</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>3.0092551878953627E-2</v>
+        <v>3.0004790944981832E-2</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>3.0115268526924966E+30</v>
+        <v>65.365853214009903</v>
       </c>
       <c r="H21">
         <f t="shared" si="3"/>
-        <v>3.3413753133385748E-5</v>
+        <v>6.5361646155887598E-5</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22">
-        <v>320</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>3.2</v>
+        <v>0.2</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>3.0088534680105326E-2</v>
+        <v>3.0001621569229937E-2</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>3.7525935346791663E+30</v>
+        <v>81.450868664968141</v>
       </c>
       <c r="H22">
         <f t="shared" si="3"/>
-        <v>3.3783320896982358E-5</v>
+        <v>8.1444316398966016E-5</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23">
-        <v>321</v>
+        <v>21</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>3.21</v>
+        <v>0.21</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>3.0084680085162376E-2</v>
+        <v>3.0000519185237044E-2</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>4.6760194829163534E+30</v>
+        <v>101.49403212954563</v>
       </c>
       <c r="H23">
         <f t="shared" si="3"/>
-        <v>3.4156976069318018E-5</v>
+        <v>1.0148383360991019E-4</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24">
-        <v>322</v>
+        <v>22</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>3.22</v>
+        <v>0.22</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>3.0080982062067031E-2</v>
+        <v>3.0000157246759255E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>5.8266790694352977E+30</v>
+        <v>126.46935173011477</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
-        <v>3.453476385390916E-5</v>
+        <v>1.2645348569324084E-4</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25">
-        <v>323</v>
+        <v>23</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>3.23</v>
+        <v>0.23</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>3.007743477797482E-2</v>
+        <v>3.0000045051950815E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>7.2604892050238504E+30</v>
+        <v>157.59051632336687</v>
       </c>
       <c r="H25">
         <f t="shared" si="3"/>
-        <v>3.4916729954118298E-5</v>
+        <v>1.575658430066555E-4</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26">
-        <v>324</v>
+        <v>24</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>3.24</v>
+        <v>0.24</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>3.0074032593724067E-2</v>
+        <v>3.0000012210066457E-2</v>
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>9.0471266510610807E+30</v>
+        <v>196.36987535179841</v>
       </c>
       <c r="H26">
         <f t="shared" si="3"/>
-        <v>3.5302920578679762E-5</v>
+        <v>1.9633151808758198E-4</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27">
-        <v>325</v>
+        <v>25</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>3.25</v>
+        <v>0.25</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>3.0070770058415741E-2</v>
+        <v>3.0000003130365025E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="2"/>
-        <v>1.1273413998564138E+31</v>
+        <v>244.69193226422038</v>
       </c>
       <c r="H27">
         <f t="shared" si="3"/>
-        <v>3.5693382447286248E-5</v>
+        <v>2.4463231734211298E-4</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28">
-        <v>326</v>
+        <v>26</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>3.26</v>
+        <v>0.26</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>3.006764190410325E-2</v>
+        <v>3.0000000759179489E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>1.4047538857888797E+31</v>
+        <v>304.90492295690854</v>
       </c>
       <c r="H28">
         <f t="shared" si="3"/>
-        <v>3.6088162796237222E-5</v>
+        <v>3.0481228900170317E-4</v>
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29">
-        <v>327</v>
+        <v>27</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>3.27</v>
+        <v>0.27</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>3.0064643040591657E-2</v>
+        <v>3.0000000174167242E-2</v>
       </c>
       <c r="G29">
         <f t="shared" si="2"/>
-        <v>1.7504311292837242E+31</v>
+        <v>379.93492953814206</v>
       </c>
       <c r="H29">
         <f t="shared" si="3"/>
-        <v>3.6487309384149801E-5</v>
+        <v>3.797910134572184E-4</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30">
-        <v>328</v>
+        <v>28</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>3.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>3.0061768550345758E-2</v>
+        <v>3.000000003779732E-2</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
-        <v>2.1811714986962375E+31</v>
+        <v>473.42807483483483</v>
       </c>
       <c r="H30">
         <f t="shared" si="3"/>
-        <v>3.6890870497732464E-5</v>
+        <v>4.7320451973457343E-4</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31">
-        <v>329</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>3.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>3.0059013683506323E-2</v>
+        <v>3.00000000077594E-2</v>
       </c>
       <c r="G31">
         <f t="shared" si="2"/>
-        <v>2.7179070499457825E+31</v>
+        <v>589.92770765846865</v>
       </c>
       <c r="H31">
         <f t="shared" si="3"/>
-        <v>3.7298894957622849E-5</v>
+        <v>5.8958048737355951E-4</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32">
-        <v>330</v>
+        <v>30</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>3.3</v>
+        <v>0.3</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>3.0056373853013799E-2</v>
+        <v>3.0000000001506842E-2</v>
       </c>
       <c r="G32">
         <f t="shared" si="2"/>
-        <v>3.3867207308368295E+31</v>
+        <v>735.09518924197266</v>
       </c>
       <c r="H32">
         <f t="shared" si="3"/>
-        <v>3.7711432124289786E-5</v>
+        <v>7.3455595524899526E-4</v>
       </c>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33">
-        <v>331</v>
+        <v>31</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>3.31</v>
+        <v>0.31</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>3.005384462983865E-2</v>
+        <v>3.0000000000276809E-2</v>
       </c>
       <c r="G33">
         <f t="shared" si="2"/>
-        <v>4.2201138956937171E+31</v>
+        <v>915.98501008114988</v>
       </c>
       <c r="H33">
         <f t="shared" si="3"/>
-        <v>3.8128531904000816E-5</v>
+        <v>9.151476636868655E-4</v>
       </c>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34">
-        <v>332</v>
+        <v>32</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>3.32</v>
+        <v>0.32</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>3.0051421738317471E-2</v>
+        <v>3.0000000000048103E-2</v>
       </c>
       <c r="G34">
         <f t="shared" si="2"/>
-        <v>5.2585857258523957E+31</v>
+        <v>1141.3876066289679</v>
       </c>
       <c r="H34">
         <f t="shared" si="3"/>
-        <v>3.855024475485522E-5</v>
+        <v>1.1400874650133936E-3</v>
       </c>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35">
-        <v>333</v>
+        <v>33</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>3.33</v>
+        <v>0.33</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>3.0049101051593922E-2</v>
+        <v>3.0000000000007906E-2</v>
       </c>
       <c r="G35">
         <f t="shared" si="2"/>
-        <v>6.5526013087836147E+31</v>
+        <v>1422.2565372011795</v>
       </c>
       <c r="H35">
         <f t="shared" si="3"/>
-        <v>3.8976621692884314E-5</v>
+        <v>1.4202380146384928E-3</v>
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36">
-        <v>334</v>
+        <v>34</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>3.34</v>
+        <v>0.34</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>3.0046878587163543E-2</v>
+        <v>3.0000000000001227E-2</v>
       </c>
       <c r="G36">
         <f t="shared" si="2"/>
-        <v>8.16504401569167E+31</v>
+        <v>1772.2407759321766</v>
       </c>
       <c r="H36">
         <f t="shared" si="3"/>
-        <v>3.9407714298218417E-5</v>
+        <v>1.7691072610144698E-3</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37">
-        <v>335</v>
+        <v>35</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>3.35</v>
+        <v>0.35</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>3.0044750502521336E-2</v>
+        <v>3.0000000000000179E-2</v>
       </c>
       <c r="G37">
         <f t="shared" si="2"/>
-        <v>1.0174271352175123E+32</v>
+        <v>2208.347991887209</v>
       </c>
       <c r="H37">
         <f t="shared" si="3"/>
-        <v>3.9843574721322512E-5</v>
+        <v>2.2034841356053255E-3</v>
       </c>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38">
-        <v>336</v>
+        <v>36</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>3.36</v>
+        <v>0.36</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>3.0042713090911076E-2</v>
+        <v>3.0000000000000023E-2</v>
       </c>
       <c r="G38">
         <f t="shared" si="2"/>
-        <v>1.2677922782627214E+32</v>
+        <v>2751.7710457300204</v>
       </c>
       <c r="H38">
         <f t="shared" si="3"/>
-        <v>4.0284255689300545E-5</v>
+        <v>2.7442223184334274E-3</v>
       </c>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39">
-        <v>337</v>
+        <v>37</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>3.37</v>
+        <v>0.37</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>3.0040762777175184E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="G39">
         <f t="shared" si="2"/>
-        <v>1.579766457161537E+32</v>
+        <v>3428.9178679882839</v>
       </c>
       <c r="H39">
         <f t="shared" si="3"/>
-        <v>4.0729810512269309E-5</v>
+        <v>3.417203973429205E-3</v>
       </c>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40">
-        <v>338</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>3.38</v>
+        <v>0.38</v>
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>3.0038896113703976E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G40">
         <f t="shared" si="2"/>
-        <v>1.9685102220314553E+32</v>
+        <v>4272.6947663954879</v>
       </c>
       <c r="H40">
         <f t="shared" si="3"/>
-        <v>4.1180293089803006E-5</v>
+        <v>4.2545207523640933E-3</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41">
-        <v>339</v>
+        <v>39</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>3.39</v>
+        <v>0.39</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>3.0037109776483065E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G41">
         <f t="shared" si="2"/>
-        <v>2.4529147815967923E+32</v>
+        <v>5324.1055253079066</v>
       </c>
       <c r="H41">
         <f t="shared" si="3"/>
-        <v>4.1635757917448627E-5</v>
+        <v>5.2959148119110623E-3</v>
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42">
-        <v>340</v>
+        <v>40</v>
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>3.4</v>
+        <v>0.4</v>
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>3.0035400561237647E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G42">
         <f t="shared" si="2"/>
-        <v>3.0565200314615865E+32</v>
+        <v>6634.2440062778896</v>
       </c>
       <c r="H42">
         <f t="shared" si="3"/>
-        <v>4.2096260093313591E-5</v>
+        <v>6.5905274297065781E-3</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43">
-        <v>341</v>
+        <v>41</v>
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>3.41</v>
+        <v>0.41</v>
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>3.0033765379672384E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G43">
         <f t="shared" si="2"/>
-        <v>3.8086584877784882E+32</v>
+        <v>8266.7770812616709</v>
       </c>
       <c r="H43">
         <f t="shared" si="3"/>
-        <v>4.256185532472612E-5</v>
+        <v>8.1990059259894974E-3</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44">
-        <v>342</v>
+        <v>42</v>
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
-        <v>3.42</v>
+        <v>0.42</v>
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>3.0032201255805562E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G44">
         <f t="shared" si="2"/>
-        <v>4.7458807163748908E+32</v>
+        <v>10301.03855791324</v>
       </c>
       <c r="H44">
         <f t="shared" si="3"/>
-        <v>4.3032599934968963E-5</v>
+        <v>1.0196019167352289E-2</v>
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D45">
-        <v>343</v>
+        <v>43</v>
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
-        <v>3.43</v>
+        <v>0.43</v>
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>3.0030705322396111E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
-        <v>5.9137315268181137E+32</v>
+        <v>12835.884447899087</v>
       </c>
       <c r="H45">
         <f t="shared" si="3"/>
-        <v>4.3508550870087824E-5</v>
+        <v>1.2673225068561876E-2</v>
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D46">
-        <v>344</v>
+        <v>44</v>
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
-        <v>3.44</v>
+        <v>0.44</v>
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>3.0029274817462193E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
-        <v>7.3689632465091313E+32</v>
+        <v>15994.496927035483</v>
       </c>
       <c r="H46">
         <f t="shared" si="3"/>
-        <v>4.3989765705774741E-5</v>
+        <v>1.5742715849473732E-2</v>
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47">
-        <v>345</v>
+        <v>45</v>
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
-        <v>3.45</v>
+        <v>0.45</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>3.0027907080889871E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
-        <v>9.1822936300286594E+32</v>
+        <v>19930.370438230297</v>
       </c>
       <c r="H47">
         <f t="shared" si="3"/>
-        <v>4.4476302654327502E-5</v>
+        <v>1.9540931966364361E-2</v>
       </c>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48">
-        <v>346</v>
+        <v>46</v>
       </c>
       <c r="E48">
         <f t="shared" si="0"/>
-        <v>3.46</v>
+        <v>0.46</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>3.0026599551130486E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
-        <v>1.1441842425799432E+33</v>
+        <v>24834.770835065363</v>
       </c>
       <c r="H48">
         <f t="shared" si="3"/>
-        <v>4.4968220571686174E-5</v>
+        <v>2.4232974694841723E-2</v>
       </c>
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D49">
-        <v>347</v>
+        <v>47</v>
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>3.47</v>
+        <v>0.47</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>3.0025349761985259E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
-        <v>1.4257413601836127E+33</v>
+        <v>30946.030047045107</v>
       </c>
       <c r="H49">
         <f t="shared" si="3"/>
-        <v>4.5465578964547087E-5</v>
+        <v>3.0017148485242659E-2</v>
       </c>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D50">
-        <v>348</v>
+        <v>48</v>
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>3.48</v>
+        <v>0.48</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>3.0024155339475698E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>1.7765831327607995E+33</v>
+        <v>38561.127945680841</v>
       </c>
       <c r="H50">
         <f t="shared" si="3"/>
-        <v>4.5968437997555506E-5</v>
+        <v>3.7129413028744424E-2</v>
       </c>
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D51">
-        <v>349</v>
+        <v>49</v>
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>3.49</v>
+        <v>0.49</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>3.0023013998798292E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>2.2137589016872612E+33</v>
+        <v>48050.124238315613</v>
       </c>
       <c r="H51">
         <f t="shared" si="3"/>
-        <v>4.6476858500577689E-5</v>
+        <v>4.5847206134766547E-2</v>
       </c>
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D52">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>3.0021923541362044E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>2.7585134545231703E+33</v>
+        <v>59874.141715197817</v>
       </c>
       <c r="H52">
         <f t="shared" si="3"/>
-        <v>4.6990901976053392E-5</v>
+        <v>5.6491800158557842E-2</v>
       </c>
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D53">
-        <v>351</v>
+        <v>51</v>
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>3.51</v>
+        <v>0.51</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>3.002088185190736E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
-        <v>3.4373194266935294E+33</v>
+        <v>74607.774755199265</v>
       </c>
       <c r="H53">
         <f t="shared" si="3"/>
-        <v>4.7510630606429336E-5</v>
+        <v>6.9427977291689119E-2</v>
       </c>
     </row>
     <row r="54" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D54">
-        <v>352</v>
+        <v>52</v>
       </c>
       <c r="E54">
         <f t="shared" si="0"/>
-        <v>3.52</v>
+        <v>0.52</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
-        <v>3.0019886895704707E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
-        <v>4.2831637531987588E+33</v>
+        <v>92967.012043358307</v>
       </c>
       <c r="H54">
         <f t="shared" si="3"/>
-        <v>4.80361072616751E-5</v>
+        <v>8.5059380638517298E-2</v>
       </c>
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D55">
-        <v>353</v>
+        <v>53</v>
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>3.53</v>
+        <v>0.53</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>3.0018936715831692E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
-        <v>5.3371506861562782E+33</v>
+        <v>115844.03041946566</v>
       </c>
       <c r="H55">
         <f t="shared" si="3"/>
-        <v>4.8567395506881678E-5</v>
+        <v>0.103817496960946</v>
       </c>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D56">
-        <v>354</v>
+        <v>54</v>
       </c>
       <c r="E56">
         <f t="shared" si="0"/>
-        <v>3.54</v>
+        <v>0.54</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>3.001802943052689E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
-        <v>6.6504992776578037E+33</v>
+        <v>144350.55068315295</v>
       </c>
       <c r="H56">
         <f t="shared" si="3"/>
-        <v>4.9104559609944175E-5</v>
+        <v>0.12614200844224446</v>
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D57">
-        <v>355</v>
+        <v>55</v>
       </c>
       <c r="E57">
         <f t="shared" si="0"/>
-        <v>3.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>3.0017163230619013E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
-        <v>8.287032396677565E+33</v>
+        <v>179871.86225375102</v>
       </c>
       <c r="H57">
         <f t="shared" si="3"/>
-        <v>4.9647664549329351E-5</v>
+        <v>0.15245046556210873</v>
       </c>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D58">
-        <v>356</v>
+        <v>56</v>
       </c>
       <c r="E58">
         <f t="shared" si="0"/>
-        <v>3.56</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>3.0016336377029905E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
-        <v>1.0326278235123822E+34</v>
+        <v>224134.14204181795</v>
       </c>
       <c r="H58">
         <f t="shared" si="3"/>
-        <v>5.0196776021928776E-5</v>
+        <v>0.18309621261292608</v>
       </c>
     </row>
     <row r="59" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D59">
-        <v>357</v>
+        <v>57</v>
       </c>
       <c r="E59">
         <f t="shared" si="0"/>
-        <v>3.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
-        <v>3.0015547198349812E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
-        <v>1.2867335022358705E+34</v>
+        <v>279288.33892847633</v>
       </c>
       <c r="H59">
         <f t="shared" si="3"/>
-        <v>5.0751960450998819E-5</v>
+        <v>0.21831556557294363</v>
       </c>
     </row>
     <row r="60" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D60">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="E60">
         <f t="shared" si="0"/>
-        <v>3.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>3.0014794088483461E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>1.603368675603322E+34</v>
+        <v>348014.70026317565</v>
       </c>
       <c r="H60">
         <f t="shared" si="3"/>
-        <v>5.1313284994188345E-5</v>
+        <v>0.25816851875854974</v>
       </c>
     </row>
     <row r="61" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D61">
-        <v>359</v>
+        <v>59</v>
       </c>
       <c r="E61">
         <f t="shared" si="0"/>
-        <v>3.59</v>
+        <v>0.59</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>3.0014075504365443E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
-        <v>1.997920397222004E+34</v>
+        <v>433653.01990028552</v>
       </c>
       <c r="H61">
         <f t="shared" si="3"/>
-        <v>5.1880817551655123E-5</v>
+        <v>0.30248136499012307</v>
       </c>
     </row>
     <row r="62" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D62">
-        <v>360</v>
+        <v>60</v>
       </c>
       <c r="E62">
         <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>0.6</v>
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>3.0013389963743402E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
-        <v>2.4895621165442335E+34</v>
+        <v>540364.93724669155</v>
       </c>
       <c r="H62">
         <f t="shared" si="3"/>
-        <v>5.2454626774271586E-5</v>
+        <v>0.35080342001031367</v>
       </c>
     </row>
     <row r="63" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D63">
-        <v>361</v>
+        <v>61</v>
       </c>
       <c r="E63">
         <f t="shared" si="0"/>
-        <v>3.61</v>
+        <v>0.61</v>
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>3.001273604302758E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G63">
         <f t="shared" si="2"/>
-        <v>3.1021854227776346E+34</v>
+        <v>673336.17432841309</v>
       </c>
       <c r="H63">
         <f t="shared" si="3"/>
-        <v>5.3034782071921506E-5</v>
+        <v>0.40239169334299929</v>
       </c>
     </row>
     <row r="64" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D64">
-        <v>362</v>
+        <v>62</v>
       </c>
       <c r="E64">
         <f t="shared" si="0"/>
-        <v>3.62</v>
+        <v>0.62</v>
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>3.0012112375205166E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G64">
         <f t="shared" si="2"/>
-        <v>3.8655610692905824E+34</v>
+        <v>839028.53869336413</v>
       </c>
       <c r="H64">
         <f t="shared" si="3"/>
-        <v>5.3621353621888093E-5</v>
+        <v>0.45623489645483883</v>
       </c>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D65">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="E65">
         <f t="shared" si="0"/>
-        <v>3.63</v>
+        <v>0.63</v>
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>3.0011517647818096E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G65">
         <f t="shared" si="2"/>
-        <v>4.8167856991074633E+34</v>
+        <v>1045493.9383645338</v>
       </c>
       <c r="H65">
         <f t="shared" si="3"/>
-        <v>5.4214412377334787E-5</v>
+        <v>0.5111207761980614</v>
       </c>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D66">
-        <v>364</v>
+        <v>64</v>
       </c>
       <c r="E66">
         <f t="shared" si="0"/>
-        <v>3.64</v>
+        <v>0.64</v>
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>3.0010950601002742E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G66">
         <f t="shared" si="2"/>
-        <v>6.0020845758838724E+34</v>
+        <v>1302765.6685662037</v>
       </c>
       <c r="H66">
         <f t="shared" si="3"/>
-        <v>5.4814030075879776E-5</v>
+        <v>0.5657398197694945</v>
       </c>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D67">
-        <v>365</v>
+        <v>65</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E85" si="5">D67/100</f>
-        <v>3.65</v>
+        <v>0.65</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F85" si="6">$B$11*EXP(-1*(E67/($B$14*$B$16))^2) + $B$12</f>
-        <v>3.0010410025590149E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G85" si="7">EXP($B$15*D67)</f>
-        <v>7.4790579250263135E+34</v>
+        <v>1623345.9850084595</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H85" si="8">((10^-6)*EXP($B$15*D67/$B$16))/(1+((10^-6)*(EXP($B$15*D67/$B$16)-1)))</f>
-        <v>5.5420279248265029E-5</v>
+        <v>0.61880766513186025</v>
       </c>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D68">
-        <v>366</v>
+        <v>66</v>
       </c>
       <c r="E68">
         <f t="shared" si="5"/>
-        <v>3.66</v>
+        <v>0.66</v>
       </c>
       <c r="F68">
         <f t="shared" si="6"/>
-        <v>3.0009894761265303E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G68">
         <f t="shared" si="7"/>
-        <v>9.3194800470904177E+34</v>
+        <v>2022813.6576114902</v>
       </c>
       <c r="H68">
         <f t="shared" si="8"/>
-        <v>5.6033233227121078E-5</v>
+        <v>0.66918260796547002</v>
       </c>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D69">
-        <v>367</v>
+        <v>67</v>
       </c>
       <c r="E69">
         <f t="shared" si="5"/>
-        <v>3.67</v>
+        <v>0.67</v>
       </c>
       <c r="F69">
         <f t="shared" si="6"/>
-        <v>3.0009403694784092E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G69">
         <f t="shared" si="7"/>
-        <v>1.1612787227852744E+35</v>
+        <v>2520581.029064029</v>
       </c>
       <c r="H69">
         <f t="shared" si="8"/>
-        <v>5.6652966155828694E-5</v>
+        <v>0.71595618002018357</v>
       </c>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D70">
-        <v>368</v>
+        <v>68</v>
       </c>
       <c r="E70">
         <f t="shared" si="5"/>
-        <v>3.68</v>
+        <v>0.68</v>
       </c>
       <c r="F70">
         <f t="shared" si="6"/>
-        <v>3.0008935758246504E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G70">
         <f t="shared" si="7"/>
-        <v>1.4470423941889625E+35</v>
+        <v>3140837.3678766829</v>
       </c>
       <c r="H70">
         <f t="shared" si="8"/>
-        <v>5.7279552997478292E-5</v>
+        <v>0.75850313531882596</v>
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D71">
-        <v>369</v>
+        <v>69</v>
       </c>
       <c r="E71">
         <f t="shared" si="5"/>
-        <v>3.69</v>
+        <v>0.69</v>
       </c>
       <c r="F71">
         <f t="shared" si="6"/>
-        <v>3.0008489927424727E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G71">
         <f t="shared" si="7"/>
-        <v>1.8031258555723421E+35</v>
+        <v>3913724.3586704475</v>
       </c>
       <c r="H71">
         <f t="shared" si="8"/>
-        <v>5.7913069543928314E-5</v>
+        <v>0.79648854300365435</v>
       </c>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D72">
-        <v>370</v>
+        <v>70</v>
       </c>
       <c r="E72">
         <f t="shared" si="5"/>
-        <v>3.7</v>
+        <v>0.7</v>
       </c>
       <c r="F72">
         <f t="shared" si="6"/>
-        <v>3.0008065220144767E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G72">
         <f t="shared" si="7"/>
-        <v>2.2468331709491552E+35</v>
+        <v>4876800.8532722685</v>
       </c>
       <c r="H72">
         <f t="shared" si="8"/>
-        <v>5.8553592424963564E-5</v>
+        <v>0.82983953427592239</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D73">
-        <v>371</v>
+        <v>71</v>
       </c>
       <c r="E73">
         <f t="shared" si="5"/>
-        <v>3.71</v>
+        <v>0.71</v>
       </c>
       <c r="F73">
         <f t="shared" si="6"/>
-        <v>3.0007660694720214E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G73">
         <f t="shared" si="7"/>
-        <v>2.7997265318315979E+35</v>
+        <v>6076868.0629712502</v>
       </c>
       <c r="H73">
         <f t="shared" si="8"/>
-        <v>5.9201199117554711E-5</v>
+        <v>0.85869467504450392</v>
       </c>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D74">
-        <v>372</v>
+        <v>72</v>
       </c>
       <c r="E74">
         <f t="shared" si="5"/>
-        <v>3.72</v>
+        <v>0.72</v>
       </c>
       <c r="F74">
         <f t="shared" si="6"/>
-        <v>3.0007275448436854E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G74">
         <f t="shared" si="7"/>
-        <v>3.4886740833234601E+35</v>
+        <v>7572243.8881180901</v>
       </c>
       <c r="H74">
         <f t="shared" si="8"/>
-        <v>5.9855967955219987E-5</v>
+        <v>0.88334453269096114</v>
       </c>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D75">
-        <v>373</v>
+        <v>73</v>
       </c>
       <c r="E75">
         <f t="shared" si="5"/>
-        <v>3.73</v>
+        <v>0.73</v>
       </c>
       <c r="F75">
         <f t="shared" si="6"/>
-        <v>3.0006908616086826E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G75">
         <f t="shared" si="7"/>
-        <v>4.3471555958326199E+35</v>
+        <v>9435596.9073164556</v>
       </c>
       <c r="H75">
         <f t="shared" si="8"/>
-        <v>6.0517978137490211E-5</v>
+        <v>0.9041742312675316</v>
       </c>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D76">
-        <v>374</v>
+        <v>74</v>
       </c>
       <c r="E76">
         <f t="shared" si="5"/>
-        <v>3.74</v>
+        <v>0.74</v>
       </c>
       <c r="F76">
         <f t="shared" si="6"/>
-        <v>3.0006559368550987E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G76">
         <f t="shared" si="7"/>
-        <v>5.4168894322097419E+35</v>
+        <v>11757477.745409319</v>
       </c>
       <c r="H76">
         <f t="shared" si="8"/>
-        <v>6.11873097394785E-5</v>
+        <v>0.92161467193268898</v>
       </c>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D77">
-        <v>375</v>
+        <v>75</v>
       </c>
       <c r="E77">
         <f t="shared" si="5"/>
-        <v>3.75</v>
+        <v>0.75</v>
       </c>
       <c r="F77">
         <f t="shared" si="6"/>
-        <v>3.0006226911428232E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G77">
         <f t="shared" si="7"/>
-        <v>6.7498598736412414E+35</v>
+        <v>14650719.428953517</v>
       </c>
       <c r="H77">
         <f t="shared" si="8"/>
-        <v>6.1864043721555188E-5</v>
+        <v>0.93610523347285957</v>
       </c>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D78">
-        <v>376</v>
+        <v>76</v>
       </c>
       <c r="E78">
         <f t="shared" si="5"/>
-        <v>3.76</v>
+        <v>0.76</v>
       </c>
       <c r="F78">
         <f t="shared" si="6"/>
-        <v>3.0005910483710544E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G78">
         <f t="shared" si="7"/>
-        <v>8.4108433232698204E+35</v>
+        <v>18255920.566783395</v>
       </c>
       <c r="H78">
         <f t="shared" si="8"/>
-        <v>6.2548261939129998E-5</v>
+        <v>0.94806796961673001</v>
       </c>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D79">
-        <v>377</v>
+        <v>77</v>
       </c>
       <c r="E79">
         <f t="shared" si="5"/>
-        <v>3.77</v>
+        <v>0.77</v>
       </c>
       <c r="F79">
         <f t="shared" si="6"/>
-        <v>3.0005609356502497E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G79">
         <f t="shared" si="7"/>
-        <v>1.0480556149742747E+36</v>
+        <v>22748277.813720435</v>
       </c>
       <c r="H79">
         <f t="shared" si="8"/>
-        <v>6.3240047152541973E-5</v>
+        <v>0.95789172377246945</v>
       </c>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D80">
-        <v>378</v>
+        <v>78</v>
       </c>
       <c r="E80">
         <f t="shared" si="5"/>
-        <v>3.78</v>
+        <v>0.78</v>
       </c>
       <c r="F80">
         <f t="shared" si="6"/>
-        <v>3.0005322831783997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G80">
         <f t="shared" si="7"/>
-        <v>1.3059577141808895E+36</v>
+        <v>28346099.644614179</v>
       </c>
       <c r="H80">
         <f t="shared" si="8"/>
-        <v>6.3939483037058633E-5</v>
+        <v>0.96592395424992794</v>
       </c>
     </row>
     <row r="81" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D81">
-        <v>379</v>
+        <v>79</v>
       </c>
       <c r="E81">
         <f t="shared" si="5"/>
-        <v>3.79</v>
+        <v>0.79</v>
       </c>
       <c r="F81">
         <f t="shared" si="6"/>
-        <v>3.0005050241215126E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G81">
         <f t="shared" si="7"/>
-        <v>1.62732351877189E+36</v>
+        <v>35321415.170064911</v>
       </c>
       <c r="H81">
         <f t="shared" si="8"/>
-        <v>6.4646654192985649E-5</v>
+        <v>0.97246805988010854</v>
       </c>
     </row>
     <row r="82" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D82">
-        <v>380</v>
+        <v>80</v>
       </c>
       <c r="E82">
         <f t="shared" si="5"/>
-        <v>3.8</v>
+        <v>0.8</v>
       </c>
       <c r="F82">
         <f t="shared" si="6"/>
-        <v>3.0004790944981832E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G82">
         <f t="shared" si="7"/>
-        <v>2.0277699698792267E+36</v>
+        <v>44013193.534834109</v>
       </c>
       <c r="H82">
         <f t="shared" si="8"/>
-        <v>6.5361646155887598E-5</v>
+        <v>0.97778431291612711</v>
       </c>
     </row>
     <row r="83" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D83">
-        <v>381</v>
+        <v>81</v>
       </c>
       <c r="E83">
         <f t="shared" si="5"/>
-        <v>3.81</v>
+        <v>0.81</v>
       </c>
       <c r="F83">
         <f t="shared" si="6"/>
-        <v>3.0004544330681383E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G83">
         <f t="shared" si="7"/>
-        <v>2.5267569744504116E+36</v>
+        <v>54843816.302595668</v>
       </c>
       <c r="H83">
         <f t="shared" si="8"/>
-        <v>6.6084545406922302E-5</v>
+        <v>0.98209293196423986</v>
       </c>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D84">
-        <v>382</v>
+        <v>82</v>
       </c>
       <c r="E84">
         <f t="shared" si="5"/>
-        <v>3.82</v>
+        <v>0.82</v>
       </c>
       <c r="F84">
         <f t="shared" si="6"/>
-        <v>3.0004309812246419E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G84">
         <f t="shared" si="7"/>
-        <v>3.1485330697120274E+36</v>
+        <v>68339603.311273232</v>
       </c>
       <c r="H84">
         <f t="shared" si="8"/>
-        <v>6.6815439383288355E-5</v>
+        <v>0.98557824148585549</v>
       </c>
     </row>
     <row r="85" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D85">
-        <v>383</v>
+        <v>83</v>
       </c>
       <c r="E85">
         <f t="shared" si="5"/>
-        <v>3.83</v>
+        <v>0.83</v>
       </c>
       <c r="F85">
         <f t="shared" si="6"/>
-        <v>3.0004086828906512E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G85">
         <f t="shared" si="7"/>
-        <v>3.9233137936530082E+36</v>
+        <v>85156389.463750094</v>
       </c>
       <c r="H85">
         <f t="shared" si="8"/>
-        <v>6.7554416488789119E-5</v>
+        <v>0.98839321125419799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added recursion for NFrond in FLMALS
Error was 'MALN greater than MALNmax', this was due to NFrond being = 0 for cells where MALS was != 0. This caused full decay and virtually no growth, making the storage terms grow relative to structural mass. This issue was not apparent in Farm3D testbench. To fix this I made NFrond recursive in FLMALS.
</commit_message>
<xml_diff>
--- a/documentation/calculations.xlsx
+++ b/documentation/calculations.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\IMPAQT\MALG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647ABB52-4863-4438-B291-6F2AB2E4F184}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F820FE2-B1CF-4743-9F1D-18A85EA5FF8B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="growth rate" sheetId="1" r:id="rId1"/>
     <sheet name="tidal condition" sheetId="3" r:id="rId2"/>
     <sheet name="Broch initials" sheetId="2" r:id="rId3"/>
+    <sheet name="light" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>umax</t>
   </si>
@@ -156,6 +157,18 @@
   </si>
   <si>
     <t>coeff</t>
+  </si>
+  <si>
+    <t>ExtVL</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>LocalDepth</t>
+  </si>
+  <si>
+    <t>RadSurf</t>
   </si>
 </sst>
 </file>
@@ -2779,6 +2792,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>sigmoid</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3197,6 +3235,428 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>light!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>79.802330225238904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.100642889799659</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.72958103636334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6947955984310044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3621038997486652</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97976033323216971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40638784376815579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16856273311015513</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>light!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-7.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DFFB-4103-8FDA-E4FA0CFD3A86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="119442512"/>
+        <c:axId val="119446120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="119442512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Irradiance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="119446120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="119446120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="119442512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3317,6 +3777,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4350,6 +4850,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4970,6 +5986,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{919F4427-3B0A-46B3-98DB-20C363C70BBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5244,7 +6301,7 @@
   <dimension ref="A1:V202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5342,7 +6399,7 @@
         <v>1.2460764239569684E-6</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="4">1/(1+EXP(-(C3)))</f>
+        <f t="shared" ref="I3:I27" si="4">1/(1+EXP(-(C3)))</f>
         <v>1.2339457598623172E-4</v>
       </c>
     </row>
@@ -9825,7 +10882,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10034,4 +11091,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D033F6CA-5C27-4411-BDC0-8FB453BBBBEB}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2">
+        <f>-$B$4/($B$2*$B$3)*(EXP(-$B$2*D2)-EXP(-$B$2*(D2-$B$3)))</f>
+        <v>79.802330225238904</v>
+      </c>
+      <c r="F2">
+        <f>D2*-1</f>
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="0">-$B$4/($B$2*$B$3)*(EXP(-$B$2*D3)-EXP(-$B$2*(D3-$B$3)))</f>
+        <v>33.100642889799659</v>
+      </c>
+      <c r="F3">
+        <f>D3*-1</f>
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <v>3.3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>13.72958103636334</v>
+      </c>
+      <c r="F4">
+        <f>D4*-1</f>
+        <v>-3.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.6947955984310044</v>
+      </c>
+      <c r="F5">
+        <f>D5*-1</f>
+        <v>-4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2.3621038997486652</v>
+      </c>
+      <c r="F6">
+        <f>D6*-1</f>
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>6.6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.97976033323216971</v>
+      </c>
+      <c r="F7">
+        <f>D7*-1</f>
+        <v>-6.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>7.7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.40638784376815579</v>
+      </c>
+      <c r="F8">
+        <f>D8*-1</f>
+        <v>-7.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.16856273311015513</v>
+      </c>
+      <c r="F9">
+        <f>D9*-1</f>
+        <v>-8.8000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>